<commit_message>
adds pub, makes title bigger
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jankrieglstein\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\GitHub\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BEFC3D-74A5-498E-9459-DBAA9BD18264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715D33F-6860-4968-B382-FE95AF9EC31A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="1981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="1986">
   <si>
     <t>Title</t>
   </si>
@@ -9082,6 +9073,30 @@
 doi = {},
 booktitle = {International Conference on Automation and Robotics},
 }</t>
+  </si>
+  <si>
+    <t>Voronoi Cell Interface-Based Parameter Sensitivity Analysis for Labeled Samples</t>
+  </si>
+  <si>
+    <t>Abstract Varying the input parameters of simulations or experiments often leads to different classes of results. Parameter sensitivity analysis in this context includes estimating the sensitivity to the individual parameters, that is, to understand which parameters contribute most to changes in output classifications and for which parameter ranges these occur. We propose a novel visual parameter sensitivity analysis approach based on Voronoi cell interfaces between the sample points in the parameter space to tackle the problem. The Voronoi diagram of the sample points in the parameter space is first calculated. We then extract Voronoi cell interfaces which we use to quantify the sensitivity to parameters, considering the class label information of each sample's corresponding output. Multiple visual encodings are then utilized to represent the cell interface transitions and class label distribution, including stacked graphs for local parameter sensitivity. We evaluate the approach's expressiveness and usefulness with case studies for synthetic and real-world datasets.</t>
+  </si>
+  <si>
+    <t>@article{https://doi.org/10.1111/cgf.70122,
+author = {Bauer, R. and Evers, M. and Ngo, Q. Q. and Reina, G. and Frey, S. and Sedlmair, M.},
+title = {Voronoi Cell Interface-Based Parameter Sensitivity Analysis for Labeled Samples},
+journal = {Computer Graphics Forum},
+volume = {n/a},
+number = {n/a},
+pages = {e70122},
+keywords = {CCS Concepts, • Human-centered computing → Information visualization, Visual analytics},
+doi = {https://doi.org/10.1111/cgf.70122},
+}</t>
+  </si>
+  <si>
+    <t>Marina Evers, Quynh Quang Ngo, Guido Reina, Steffen Frey, Michael Sedlmair</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1111/cgf.70122</t>
   </si>
 </sst>
 </file>
@@ -9198,9 +9213,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
@@ -9272,7 +9286,7 @@
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -9281,10 +9295,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -9383,9 +9396,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D20E5FC-A000-49DA-943E-3394DF221AF3}" name="Table2" displayName="Table2" ref="A1:R272" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:R272" xr:uid="{4D20E5FC-A000-49DA-943E-3394DF221AF3}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R269">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4D20E5FC-A000-49DA-943E-3394DF221AF3}" name="Table2" displayName="Table2" ref="A1:R273" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:R273" xr:uid="{4D20E5FC-A000-49DA-943E-3394DF221AF3}"/>
+  <sortState ref="A2:R269">
     <sortCondition ref="C1:C269"/>
   </sortState>
   <tableColumns count="18">
@@ -9415,7 +9428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9711,13 +9724,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R272"/>
+  <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" workbookViewId="0">
-      <selection activeCell="R274" sqref="R274"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <selection activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="60.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -20851,6 +20864,47 @@
       </c>
       <c r="Q272" s="27"/>
       <c r="R272" s="27"/>
+    </row>
+    <row r="273" spans="1:18" ht="50.25" customHeight="1">
+      <c r="A273" s="5" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B273" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C273" s="6">
+        <v>45800</v>
+      </c>
+      <c r="D273" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="E273" s="5" t="s">
+        <v>1698</v>
+      </c>
+      <c r="F273" s="5" t="s">
+        <v>1984</v>
+      </c>
+      <c r="G273" s="5" t="str">
+        <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E273," ",REPT(" ",100)),100)) &amp; YEAR(C273) &amp; IFERROR(LEFT(A273,FIND(" ",A273)-1),A273)), ":", "")</f>
+        <v>bauer2025voronoi</v>
+      </c>
+      <c r="H273" s="18" t="s">
+        <v>1985</v>
+      </c>
+      <c r="I273" s="7"/>
+      <c r="J273" s="7"/>
+      <c r="K273" s="7"/>
+      <c r="L273" s="7"/>
+      <c r="M273" s="7"/>
+      <c r="N273" s="8"/>
+      <c r="O273" s="5" t="s">
+        <v>1982</v>
+      </c>
+      <c r="P273" s="23" t="s">
+        <v>1983</v>
+      </c>
+      <c r="Q273" s="7"/>
+      <c r="R273" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -21338,11 +21392,12 @@
     <hyperlink ref="H271" r:id="rId482" xr:uid="{016BA2FB-597C-4FDD-B2BA-E53E0C4FD788}"/>
     <hyperlink ref="J271" r:id="rId483" xr:uid="{E9215BA0-45A1-4652-AEF1-A00C1295EFDA}"/>
     <hyperlink ref="K272" r:id="rId484" xr:uid="{23479075-357B-4E14-B7E5-34B750AE71BA}"/>
+    <hyperlink ref="H273" r:id="rId485" xr:uid="{1FE003AB-2EE7-4EEB-9167-234FAA90E3FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId485"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId486"/>
   <tableParts count="1">
-    <tablePart r:id="rId486"/>
+    <tablePart r:id="rId487"/>
   </tableParts>
 </worksheet>
 </file>
@@ -21603,15 +21658,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bcc6a80-9cbb-4ef4-81b1-0de6e4d1e31e">
@@ -21620,6 +21666,15 @@
     <TaxCatchAll xmlns="2f19b678-e8b7-409b-86f9-6b59659c2b24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21642,14 +21697,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74FA3D6-0E8A-4136-B53D-83DD582CB2C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -21658,4 +21705,12 @@
     <ds:schemaRef ds:uri="2f19b678-e8b7-409b-86f9-6b59659c2b24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added teaser, funding and ack.
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\GitHub\visvar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bauerrn\Projekte\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715D33F-6860-4968-B382-FE95AF9EC31A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA85FC21-6949-4652-ADBE-073A7BB37AE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2449" uniqueCount="1986">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1988">
   <si>
     <t>Title</t>
   </si>
@@ -9097,6 +9097,12 @@
   </si>
   <si>
     <t>https://doi.org/10.1111/cgf.70122</t>
+  </si>
+  <si>
+    <t>Funded by Deutsche Forschungsgemeinschaft (DFG, German Research Foundation) under Germany's Excellence Strategy - EXC 2075 - 390740016, Project 327154368 - SFB 1313 (D01), and Project 251654672 – TRR 161 (A01, A08). We acknowledge the support of the Stuttgart Center for Simulation Science (SimTech). Open Access funding enabled and organized by Projekt DEAL.</t>
+  </si>
+  <si>
+    <t>Open Access funding enabled and organized by Projekt DEAL.</t>
   </si>
 </sst>
 </file>
@@ -9297,7 +9303,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="20">
     <dxf>
@@ -9428,7 +9434,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9726,11 +9732,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <selection activeCell="F275" sqref="F275"/>
+    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
+      <selection activeCell="B273" sqref="B273"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="60.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
@@ -20896,7 +20902,9 @@
       <c r="K273" s="7"/>
       <c r="L273" s="7"/>
       <c r="M273" s="7"/>
-      <c r="N273" s="8"/>
+      <c r="N273" s="8" t="s">
+        <v>1986</v>
+      </c>
       <c r="O273" s="5" t="s">
         <v>1982</v>
       </c>
@@ -20904,7 +20912,9 @@
         <v>1983</v>
       </c>
       <c r="Q273" s="7"/>
-      <c r="R273" s="7"/>
+      <c r="R273" s="7" t="s">
+        <v>1987</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -21658,6 +21668,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bcc6a80-9cbb-4ef4-81b1-0de6e4d1e31e">
@@ -21666,15 +21685,6 @@
     <TaxCatchAll xmlns="2f19b678-e8b7-409b-86f9-6b59659c2b24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21697,6 +21707,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74FA3D6-0E8A-4136-B53D-83DD582CB2C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -21705,12 +21723,4 @@
     <ds:schemaRef ds:uri="2f19b678-e8b7-409b-86f9-6b59659c2b24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes replicability stamp to path
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bauerrn\Projekte\visvar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krautecn\Documents\GitHub\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA85FC21-6949-4652-ADBE-073A7BB37AE9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19659FF-6B2C-45D7-B75B-85858637CEB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8721,14 +8721,6 @@
 </t>
   </si>
   <si>
-    <t>&lt;a href="https://www.replicabilitystamp.org/#https-github-com-visvar-maicov2" target="_blank" rel="noreferrer"&gt;
-   &lt;img 
-style="width: 20px; height: 20px; vertical-align: middle;"
-src="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAOEAAADhCAMAAAAJbSJIAAAAilBMVEX///8AAAD5+fn09PTv7+/i4uLq6ur8/Pzx8fHl5eW8vLzz8/OamprOzs7c3NyysrKkpKTHx8eCgoLV1dWSkpLAwMBeXl5VVVWqqqpOTk4WFhZ8fHx1dXW2trZGRkaYmJiKiopmZmYxMTENDQ0fHx89PT12dnYcHBw3NzcrKytjY2MsLCxISEgRERHOAWsxAAAgAElEQVR4nO1dCZeiPLNOUEBUdhAUUFBxa/v//72bSkjYEbtx5v3umTpnzrQoIUvVU2sCQv/oH/2jf/SP/tE/+kf/6F0yEFr87T5MT4qsL7PQvN33d3xaY0JfOaEgS015Jv3t3v2OZMtJN7hKS9ykvbP2/zeXVQnja2s4OGxfAgoic/63O/wWSdZx0zmSW1b5cK//Zh8a6t/u+Diam0H3QhG6Vr+y27OwNf9271+RqnvHBv+x/047QteLgc/n8xX+3uF19ySkxt8exAC5ervDyc6zFQGYimsb2oz9vVinl23XGL/Tv9T/F6QdmsCyT0NXIUJph1H2/C4u5uw/cp18YZP1mifZrjXIp/+3h9MiLat38RwvJSS5VuzGOIgPiW/rumssVBXNZjNZX8E9iy0Z9jXWE13207wxxvN/SyLdOmbkS3JN8wh0OpY2fKfqWsDaGx2hZROgnP+MmrQfVdbM/Bky1qS3sT4W/F3LOZ/26VJxnfoY/xugY1el6HxAaGbucL6W321HTomy8JGbfpF2CkB2PtHhN0mvstbZR3pEFm+5+lljLlE1mS/NImyxBm2kIu2vWq6yKkYXPDauSlTc1v5ViwsytghpBjS581FC9On172HOKoC5vjIl4aOZg50pBMe840xH/h6vD9DwBu9mf0keiZvwRQzpHPREiOZrK/ohc7bIiPHNV306cynhi2+cTtTyWwQC+EUQYXfCa1CHyykbV82jh1DFEYknbX4Muev5nXDomTzcQ8YWp5M/QUKhKXnlGLd/1L3SiOzttTPeP3Cmans8GX/WiCxhMkvLMeqfeEg3mQXnUIDxsKN86DkEu46yWuqjyx9SHJIw0R5zycL3t3X7G6TE+IFKN+v0qbmskSyed9XkM04+/bht5srCLN//AWF0xQAddMDB7PNPtPFWTUpO/fTjDqXcS7ePL2BBAda1b7GMnxXGjD8nJwo//2P4beGNEgnh+KQwCljzyFitDz6oSdod26X+/xi2KUTH4+hAoHSJTjv3U4/pJgenyo0P8UPPZmGmbWZpc+WPLiAjGwdImDgfUf4CRNOF86lJHCQZ71YiKfA7H62TDN62SaTxA+2PIGIJ20JtTG6JK7zl9ex0/msRImNW+hsTayqpCMbcEhlvp236XTI/soqze9HqzMfxlA3/hIQsTgk3HKYtBac/bGJmmBqyz5Ru+fORrk3b/ZnuFow6nV7k8dBQt3+iJRaSD0z+bZUmn6CN+YNRGty+mcqA496L5eK3PV3X25PRLYilYIX4axOZtu0nB2dzLweZp+Hbkabi1okgwS6aOxg4fOvGWfpkd0YoYVOjGKZimqHpyxAOl/S1yD2t3+sTl8VJQIHrieg9GVwtYzrLli2z4H7qpG4Wp/M4sdPNNtjsz0G0diXZ94i1+4WP2VsCYP5sZrpIOrOmAoSzN26jnB0nxH3slbOZb1obfIt0NNNoh+/OG7FfHr/5vc4oMgg5ym9jb5GQ4ZA7fITU0Im8YftAtg+xY0tId04wyPF5Qx5LeZHceknFVN2l/XjgWmcLGJ+7TrxxN6jh8+ZpiFpk95GL4s+Kub+P7VY38aAMmbHR7u4qz+E/13sLIf2vp4uWEJDZj9LkcT6roI1ixfn3LvqBgixAXTffS+W5wQ+yKZqVWxBcI7gzYh1V7PDpN/Wn0Dzvob1Q9dEMj5KPJDUPpHNKlv1QODziucxAnd9e2wFEd9UKrK4MEu9vhVaKFnboNkagtJyi95xohHceUicDe0gGI/G166Bni2Ltjj7DCJtal28YSRpHq/V+xK8hqRnPlOzxy/iUdTUp5gQvejrTY3ymOsZAqpk9NoeNjvRvsiDjK6sKPF7LI1BmRtT2iUDEOJgYJvPsKucX2tz2KEQQPSOZXsY59TFXCcIexj6IevVEJaMRxhpMekTmZBprf36NkUOtjO6v3XCL3e9jRMDBqGRugGSJSOTIx6jU6bWPSvbavgUAtJE3gQlVkIMVCHwdO0LqLLEOvKLqabv6UfHwOFgUul72X6p6lUDMU11tp/RIjfMSpKSeilGsbHcjxvpaAyP+qzU6iqWEZY/jnsFuiNFLV1ohE5mi5DZxtD0Kqasrnq5ZdMECn0gCARmcdA6Q0Ti7iLmrs8fjxe9cCu2bd8zycSSfVOBUajssI7pim0RCK5MBy6NndPS7cU/IQgf7/iunF3SmOwaM3ieDCaNn08k+O0S8tPVtYGAljWpfMqzbA70yLoGRZN37TD5IwTav54xIP6SeEuoKgUe92Y0L+0Nr55cdBzWvLD8VXzS2GKyWYE06bFzGrF1G/l0SwIVXlMXgrRloOWwfgJ87/9QAJejy1QI0tePvoXHV6ZuA5PlV4wbe6GSIq0M++DMY4MJ/TjWkkiTXOx9vVzv2idILM7zprovvodn+dVVjgkGgD6thKxbweq6PsVnfIoPh5n29IF7jW0MrKLu9tNwKxwvFg0YKWHW+PO0AF+6aLAA+paGMZI9F4o733rH004tusdKHjTqo7EFM7MWULLqwaGDiuoHUViJq/vekO7cIFvPYORhGNycSRcbZ9YW+KBJpRjoor+SRrjodyLgWZcgjlE0b2cpoDWGXYSV1nNb1gu5BdsjxNsTODRvmC0GkgU4IHw4ZPy54NxMNUPUzeOIJNkDJVjy/4xlqrVdK9H1DY+y/Ut/3l1Zp3gTBcZPjhPDXUPRVYj/2w6GV1iHAGExTjMG0ekbMIsUDJXXOseMhddkcZFDV+KfbtlTri7oPtUXg9PVTEU5Gg9OQ45P6+P2mCCW5He0EWwfiJulpFVKuiRh7B93SZhS2tryGPWjWMJxZ+0NLSGZBXvzSHZRMh+mCcI5UU1bj5jDybd8Gqi5H28Gh8KeIRzRQBV9EZ9BxQKWQ33iz0THwLpqHbHQXfSZbKR2J1TGUg+F3YUsnjATbPf/+hLYDaMpY2lGGHF/CTuj2cx41LGJu6vgeh6qqex0jEHS8JTIywmItN3xNO7lHPYo1pHUpvWx6or9ZOFF/D8ntdrL54fBsxo0RkpB8qftC39mmQ7uf0gRSonvCzLwoq9uYrGiYtdtv1rBs4RYNKJQFQDf+SUEGsTdp8zfi1qpo3xzLVxnBbNBKYzFmHgMW8RtjWWE1UfoG/e9Nn7IuWMkAzlzwETnvp7vdAxtSHPqu6d2x3IIWnN/Wp9bFKCnLdwpNVmrq6t/VRYQK8e5uFOkOd9svZQYET0bHJPlNTLzztSK2uZ387vWq0cmqh9sKS1zEGYFty66WwSlr1WfWFLVdykDwYku4afNOfYFiplR5Z6ZC1EJlU2UXyGT1j82Z5Lfw55uwG0N8W+LuDe1wdyqCQfbBP/X2l2jhxB5vri0sql/PdPOrVd8zGmvn1gjN+nbLJp5xRuRoqhBMwCLRpZQ39umLgs/1S782hztP4yr3VNuiM7YNFVCAu1a1yRX8tLpaz8igT1GpGxsD5Hk0waZ3vK1Aa3mffOgu72NIekX9uWPCxuFqjLKXEiYz91BCWnP/MyfIV9XEkfBZBh0T/FZBmZlZUS78KkVXIXGZ+D7UcWcAkDVsuv1IGpDxxy8t7mJ4x1BeoZnKMd5qMWW0cnBaXdr1jEWGBCwK48vDNezlhhvlOiFxpQUO+qIL71kXDKe3ToXoK9N4UcWiLanxHngu7B4qtZ4jtbc0g1dbNddEYJmrfgEIdv0+MagcV1RfpSnNwR2J6EJSpf785JrwRzak7DWLsJIfbCAXvKYgY3/jqBhaXyT+nF6LiRB1B2LBRJxh8czpTrbGyOmylR9O3MUiRkmH3clEIlf6E4ZHHEv9AXzToVMfExZaJBwU7gTOM/Zn+9wPNsCQ9RTEjD9ZTEbVR5Aqq8TBzqiOMMA7PgdX1GXbMTb2lr3hC9Kc4XVXCEshlXqPHlTCWaqwlS/FGnbp+HNxiAKxBaE6SsiO+L7+GGHWCbQ/VpJNBOiFUaTCnusmMVbR07RvhBFp7NwRJbZhP737hNQCmNYJX6xvhqdBkefLmlBzTku9A99lsZBxARoNmeCXhb5YV0CzRJrwofgd/kUx+KBPDOdkjqWmEl4xb8ELE7A9qU73m67rkwFHVNP4B79mGWU4J5pNmGCicr6BiKJGmF+QKzuFqsa8jNqVfUWjUm+l+rLlXis8GeQiaSnQwcQNii/tETaNKgvOAjFDbkiLTdTNfKcrM53GIUgtrRO39lCJPLTBb4y34n5tENRtjEUIc3a9JAmOLlVtZbbSDOzbezUr3XyKQksrSldhy++r28AS4U8DoqkdDuw+I9zLzYIdoEEj4svM2n6jmjCpPS/ukcKIdgjSXvObg3CV2kk+T/BtORP1+Z2ByH5VEIT2xvqqG18amLn3s02kvV2Q4O3PdIYYnCawl74xQgYL/QYLQXA5pWpU9QSnaRBjqA+wg550hCcwAoSfWnXQmH2OAYM5sggVL9hZ88TU5R2x3MIOeho0K3Hf7mHTW/0nlLcG3AaH+E3BfD5DHPUtLnqNmojuw3XWbO4E3gvIKndQQhfEIoob+QUTHEyPcAhVtU5DF4RBLY1DJlI2cV7T+sz7HahGyXEA82Rk+Nx2e6okdV0UcieucDa1cVS0d4jwacd/J9xHvtjEcd9vZA25DFHqEOTgeniAwEyq4Lrlxmy2E+pD0gV4m0Rn+S6AEhlnJ108fOz03oVxIqbaFg3nHr4emP8RzvnAxWILTJF2maWW35QsqCbN821A3vOm9c2SardZl+skUZ2Oo9Cmrt4dFqAMMx/KGBC+z2oPipaayphWMIfQJULAtlt7JgSvxAG8YUvbdNak7/r9itWO7lAiXFdDXDbzRxs3jR2pOL0rIkw9OxQMhQLhKSxRtfSDdpSaj19eYVOwL7iBIaagWd7Lrqbi8zYvHtEMqVSDisah6nvW1RRh9JpxyozazGw4hz5Fk51nq8goQd8ql+o4a8UFwXGPykjQtt51ofcbRpXTuCis7CZwEv9hS0s0DavhWtdteygKqt7HuM5bVwrmZqFHGTwiLO8bFaxKUUXDV220/ZZNU832Kbpa6SCjRm6hSMQI8Zrz3zW9GSKH8aI1qxiOz+B/rWG6yINrtzJW8w/czFPm0MoJPFk1zGumWIxahhnvTETjFnUqusoxsQwY1X/G2ULYHIL5m8Y+sdm1rsRUqTAzEM3oUNfujHlWHgjnHJH1P6XBGo4jYwnMipILGnmviqCTEXZsmWdsLPhPxO4b1kXBciJ1LjC5Fr2du7SnqB2MbOeq6nqBPVdbx2qyheqi/VoiuHnpON8xbiSEKhGGzaUVAUQ8OiI+tjQdkOQK+eR8KvRqyWuSyVXxzYN521bt4eaYz42gcNE6TMQD3yARktQg5NH5J9A2rVn1jeGtzMLdF7Ipfi0EUbKqCk2waV5v0vV4hzI6bIfOUSkwlM3yEi5QQ1yKqSGQC4dBqMusPgxLDPeK6muY4W22eeRguz2dW7OCtZyNsgSEs7Vw4OtiLbhAeLQETeVDRRXE7CJ0q5JaJVi5S3Dvxv1C/s+wI3CWDJXqSDW787yUGBBIHPvqbFrhA6FoRae4aNbDcGJpS+OoER5gonNM5erF7whWx6e8SturmC6SD1bJ9z4IXeKgxDvczgvFwoSZ1U43avjplGojrHRC6AEBVFnjTkalTzts/4oTXzc05nqirHWUUGzPYISlFCpMp2dLkAeWv2kEb79tXTxMETrn4rdCNmzpvZm/KdsvmymNRLFkXFLqOW4xFZ2HYwryBIOEVGKv/G7o4qnkUeC5b5NYRlr8zLoaOj2ClcpFzyyBs6twkUmdiStWZ+kPB+vqMylxc6UegCgG7rZZqU41I+1Z+8Yrewdd34D33Ht07Ld5ImhyD0XnC+pK0DGtbeGKNFYxnF8TUfu2T8UHLg+vX5v8uVP+WekShF49tB6qGSuIPjF4pAmXos7tW5Rd6EpyXKmigZBaYSTwC1n9YUdLxm/Q3tKI4SXgsaolQKk66BU3cDqxPVtify+nZakgyqbEBFTQVPxO6BCOpq14eMMqu3ckPTAzpwJrQQCExmYfbOGr8nMA96u3Hq5GQchlt1BTwjNRKqBYtiUs+Ar2CuGkyHJMyyxvKy7g1MHu0l2WcoBNhy71D+6WjedsgqtMRT7Kdue9dcq9ipPG1RTnQxC+xuirz5mXl8SomZseV6aptb3gNWM9QgK6LnW/YxrCxxrbtVAd4ZU8ou3etR5Wh03uuYgV2ZU2bsUacCtfN0ddImwxcwLBxHy/KM1/WjOkH0BgTpHN+qdilwVla73FznyoHdaRZpifW+P8s3MSQcBKQEOov8pqCDNDKEAfEqoVHE9H1ATvIJ3Dzk6FFHo5GDJCOOe+Zo/ezL6qj13k6waD9WYZHOcovkpKqfsrDYjAZGU1hLsu4kz5phVFIhPbW5YIWpUMz9yALtyENf9LxURerqeGpk7trpI5gYRMrOopLpsacPBNO4VTa4w/vlIjkYpf9hpkgFU56lnJM2EMLcnIX3evdVCxlK/Yr6oXZ7izdi7iTFcssPAklZCznN4aOaqBCq7Yl+UqlQHnrG+EJsyS3VX/dVtrSKFgve88qFjL5u0RxjjpWMNK6IeZAkIZqIXZjncA763syKwW1ysnoJSzGQNgpZtzqIDTamfU/ME2XKDlg85V31F/65gJSS2IR5iiPVtVB+9QnxUbL5m+tyjrtUzT+iJyXJHqjcuHbvVdAGkKBvy6YqkeY8sl/g9dPdhd0lfOs44ZbNS0RUQG3JT0WrlQYTxxptB2F+zo0hN7VBjbOf2aCd1KBhI6xQNgSaftBjMiCbM0m0PQDz4+lxKGoFHvaY16I27J1gQbDX5o5GbYxQamEHRk/WzXO1TtB4HBdXXe/3qIRSH3HrOCiZ1ChudT8+ZOMzsYffXtDwZiFlUt/kSUt9OwcatBfVUubJTGpkWZl8F0CHylpuSbX6uu7Hc878VRrzCewxC0VaIAeoANcS/qGebbWY/Fz4i56fUQ3h3vuM2R0U6n4islDsueNRKnpyKEKLR6hbUrPMFd2VocRkn6oq2CYrQkC+GyFwrEpTMUAy4OHCma0bvrPyDrqhX64utZGwrIROmjNWr5Lk9mvIisSVgR76jSU2gorEu6HKt4mGSyTAu65T7V1SqaYdhW3T9AmxqzjcJK4DeKQPfCJxLf1AOlDeZ3cbG8ZYFZxfApxc5OohZLLqPmKwKq9IQyVNv1HvjoLRtpMO24aFdklhNrJVTEm5uxbiwqh00QgWtp6zcN3/pdQtjE2n5Vl3lwu266PPeE8r4jX0IuvFkhDFBHki/0rIEjM3DIetUsu3VIz2D5qN+RPQX+5419jWXMQtKzUpDEjETVZw+YlbgXS2Mdylfgry+rey/E3rj1i6GMdYYNTXVJOuuWTp2X8uvf2/oqiqE3rDz+QLva9vAIO2hjEoPMokv/PPQdPiFjeWArevJdFHo3v5Do4R6cTqKC6tZIjAvUzHBQjeoI5SMad1vvVGnSoa6gspC4evTFFthxB7YeX6z1wE6R9MEkq11r4eF9xdAXI8ya3eIga+DLA8e2XJgmwjY9ABwZy6h5XweFpaEawHus2E7tezy8D2eGST/7d4fu10WVUesbMvBFqcIEIrZMYxGmvdpUP3FZ5Jd9qD3lQxge4abAMQd4M/HA9o3tlwf6eZ7RXdrMCOsM3tulwasam4o1brn+zcJZ7vWxkUvLcyUC8UoOofWM3LhiZQGbF9viKal4cRlQ9y4uELyDjWOoXS8fzimrd8pqHS5XYdPisEaxdBSGB0JJGvJWRPQAwx8He9yRDOFTGtp0d8iY+7vr+I7wo1y6UEIrKLU+PdBXc/n5CB4inl5uWgEWDnuCeEdwoeQdANluPf7ACbqPqJ+Vj/Z8zye8STY911L0TVznQVqKjIv24awdwsZjPhuENxHuCsxvD1D4uSHIf43Nd84EW2bG0HEQKwJDdKa7di9LbNel6JwgnRpuDpjsGQyncV9HYTpkjQEnY7LAAdYac3B21xC1yjC4zu8eyU/b7b/pEBQxms7Kww1xgzPRj7TyjRnRQHcBRFUZnq+fuE3AepCL9KiQBtVU6mZJWlqFwJuP8P0DpYxEHtyhDfvtgLr3JhLekirKoYPXmfoShucq7HdiaVGLyVSTMN4zOFLN3YKbdjR/ctbLPCOMNHBAgI6LUEWPNoHyorKLHdsNGGYwIJNfHINjE66301IET1BvpC03UAPMo9Nv03pJhHrA9U2jAhh72s+IqcBttGMXMxS3y6r16KmSK8knMig44uq4SKJuCz45Pz/p3F6j4XMSrgYLmfVVcEOJOre25reuXV/sO6VlktUckBNjlMDIiphXQqyEJWD48T3cbJGBBkJsCICi0M69R3nsiDNddHNHFjFrIQG9/4ss9hB9C9acbU6WriJlSb2W6Lfn8O/1ZiFlgzKvUOi9QpATNK11th50VdjI7nUjoGOIxf93NIeybGDo7+j3p/CnmRSvvgcAyoCNXED9O5bIAq4a61Pa+Tzehs89W61LAjOHBo5cqgrzwxSvTLPPxEUfPAxzcyvWZ2A219iu5JnpWnhBkCAtzEpo8V7W5CdwuMw82W9vdnAxpnnPjoShEGRw8zheMmNq8LwZzSxrYh2x6bEejVq3j42pEWwnkj1q+E34DppcS14cF2yvVdbRwYV2A3TXM/q7tGupoMBqyHd/wMnqMoWr7aRv87v4IP2DRhDsegX6HvoRMna+waR1i6o508J4ydACX3sT/pkP53M7W7y/+8tpj6fzLKKpo8E2lxglVI0NH4OwJ8qyKFivDmRX6O5U8/HRSjuigPdUh7JPUBRba/LXs6gGBF+H4fia+DRf268qKEESaqj6AdTkseVNHEPYRkCDvvFPDbIhSjIofUgHf+NjqLU4RT1HDAgiLutCP1bzeuGrGo3ckwlu0ml5Wh95NYsVgLn14qifK/O0rdML8dAAiWr5hGPfthhK6xmUstyhvjTWPvTady8gbBW/OCfGxIj18+WppTciiD6uJWfLD3V79Bi6kMilQaT03UNAxpOzgb6/ciWxpZxo9dfL9gibEp7PO/dbZxVnfUvcV8nnNVlXtPzVcUoDlDkAfUPWKFCKaQopN0ecEXvGsCmsy7W9VTS9zYPvkYFUgmD5zMg/8q43F6ztl6911rDN4rZjTjG28KXHKmObzr/i0LaDB43ox4XWO9C2b9O/lFi+zVfnES8heW5ZvH7U6chkLuYgs5uODZJmHs7RglWhHr2K1gM9lCJn6mOEvQdNjL9kjgSrzMIcxUYuHGpOfhwU6UsfF/rdCmDBlu0yMiBg4D2y75O+Tta26dS9tB9meFmo6HGnOhHNtqiUFCQO2DNXR0eqTy3Sc5Z0eAugjM4L7evtYfSSfZQNUEOvA3LBtkivvDx0ltECIlVlxiGRr1+QylvQhGHm9zGCdqPCaMfTGKTGM4MFzF6BKAIeXRVsNva09JR48UjjpoypY11j5+FtwkFXD9g6Is+b4K2IUoxt5U7U2wiuX2CrMKHHw8CdopeWeKmlGyGL7ewur19QAqxyspH19duT50PiW0Kv7TEmfP5kAcLzeTwIwOtpkngpa4q2EvlBZdt/LhanFRg9W0ONh89WfkHufY30fTISN1JeGfbeMx2cFB7G/l6YLTtpzCuHloxbVH/zw3VUzW2M5luA7lFWvLR3C1syfe9BBqJRmie8XqpIEA4eKlT2kALSEimX4Cdeom/qiKrjfGRgFVvcUX/XpFIJJBZ8zdPAI98XKYER5xChTeL4rYWUiAjb9HY8+h0SzlZ7r3fdRIQ+JmC6H+v8yYHLYttKfLLGBqPcOCc+vJ3DDsnRE3PB/AzBX76uM8Z3/Wug0GqAwvx8eMU/kmHF21RCCmQ29Edzz2c/JXzvCD79MqpXFPe+PUIXP2BdbOlrkxrd/rHqrmfuEgJ0Fs1tPt6I0C3pmXpv6fpeYio1t9+cKWraBmvyeDl8EP9t61mmmSTJknVI9oI8AvdENsCuTP33gjxL7HKHdYIXa/Cm3jsXWUrgvh3Wj3tLm6kLw9X90Esv21LTKUlKoNMhzJa9ib0JtjmMvnIfRxEogQ0d4uItw3Nu29aDBybv20dkmTqxI5B98Jwo3hS7+D3Vf9ecTbDYHzjRqf4ExCHiRAyNtx3d+ezQDJNfCjVtYSWwfhIcJ4YdDznspgo+83LXAzJ+oMulxcqN0/CGmUX/QFlMKFV/6FCaxT6In6j6/j7y7QPp6lfugzybGdovexXicMUHOGF6RLSZKlO/D/tNMnGZIps0/yP4wlsNFUR8nFRsf2IFgbgNSNTZMfhQhPs1WYkqBjj5G+z5EG86yqaT8PdIxrrME9LTvcVOkFK0nYGGnHwCR5LIfaWfaH3Op29HrKZJbIm3yTulH1tBoBVXGmfVwPs/L4xKjr+7tyVPRhKvZzvOF/dfv0z5HZo7ccGhsGl48kRzhXja5qQSYZwgdjiSLLxRi8NjTs/TZ3GO5/FPuaFdd1O+tbKflCO2y/2WXW/unJTElqybQkzyHud2UlIIrpTFIR0HiU1NuiiR8pDmjX2r6c8ptfWu00Q+SmXG20BhbE3zhtwesnCElHLf8CcxpkqCZ07bhLDq42OSEcJblMsEe98m9Q8Qn9WNgwOVoNwn3kIKfsSeMAkVCufPcSgntkNvAwJioXmAw8khZwmpHp46We/xRK9AG08yqEZ2mvy3CZ+iSS0A+4yXyC931H39DZ9tYcDJO8fCTlQy/JxOFXuZi4zKjoDNn5PABm35Xq7lera64MtyskEWdddF61O1+j4Z/HAzMt97G07g3U/BrJJV3fw4Ufb8h+RXS1FzA8nOFJZcpc23gv2foVpB5terd0CPaG8fV2yY7E8jaCc1XnK0/UV9vmZBdlbw6LTl1L8gqfkip/wnm7dWOj/X8MT+9z5qD75JUtjcqneLrHck0k0bZ0vs/mbQspuMjhNZMst9KUeGjIxt896uV9PO4sQAAADISURBVB/8B0j2WG2qXd+8Fxx8eb5YzSSpatlJC9lehumauNSrtDG88D8BL92kAwo2s03iZWKn6zEPssjzTqfqq1/D2gEL6X9J+jrJWDdPucqd7nO9OO1Fxfwt+jNxkV+T7TROQ60WrPZu0Dyv/2T07tekhFnZd6e6af3SHBnQxkv+88zZQfLSi3N6guppYITnX+4u/fvkJnLtyKQiPJDD2BJt/tfyWFPT3HBt0zp4nq9by1D+UxGlf/SP/tE/+kf/6B/9o/8n9H/QbeJhBRCNOQAAAABJRU5ErkJggg==" alt="stamp icon" /&gt;
-    Graphics Replicability Stamp
-&lt;/a&gt;</t>
-  </si>
-  <si>
     <t>Mixing and Matching: Instruction Conveyance for Collaborative Tasks Using Asymmetric Augmented Reality Setups</t>
   </si>
   <si>
@@ -9103,6 +9095,12 @@
   </si>
   <si>
     <t>Open Access funding enabled and organized by Projekt DEAL.</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.replicabilitystamp.org/#https-github-com-visvar-maicov2" target="_blank" rel="noreferrer"&gt;
+   &lt;img style="width: 20px; height: 20px; vertical-align: middle;" alt="stamp icon" src="../assets/img/misc/stamp.png"&gt;
+    Graphics Replicability Stamp
+&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -9732,8 +9730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="B273" sqref="B273"/>
+    <sheetView tabSelected="1" topLeftCell="P258" workbookViewId="0">
+      <selection activeCell="Q262" sqref="Q262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
@@ -16996,7 +16994,7 @@
         <v>523</v>
       </c>
       <c r="F182" s="5" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="G182" s="5" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E182," ",REPT(" ",100)),100)) &amp; YEAR(C182) &amp; IFERROR(LEFT(A182,FIND(" ",A182)-1),A182)), ":", "")</f>
@@ -20432,13 +20430,13 @@
         <v>1909</v>
       </c>
       <c r="Q262" s="7" t="s">
-        <v>1910</v>
+        <v>1987</v>
       </c>
       <c r="R262" s="7"/>
     </row>
     <row r="263" spans="1:18" ht="50.25" customHeight="1">
       <c r="A263" s="5" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B263" s="5" t="s">
         <v>1208</v>
@@ -20450,20 +20448,20 @@
         <v>26</v>
       </c>
       <c r="E263" s="5" t="s">
+        <v>1911</v>
+      </c>
+      <c r="F263" s="5" t="s">
         <v>1912</v>
-      </c>
-      <c r="F263" s="5" t="s">
-        <v>1913</v>
       </c>
       <c r="G263" s="5" t="str">
         <f t="shared" si="5"/>
         <v>aygün2025mixing</v>
       </c>
       <c r="H263" s="7" t="s">
+        <v>1913</v>
+      </c>
+      <c r="I263" s="7" t="s">
         <v>1914</v>
-      </c>
-      <c r="I263" s="7" t="s">
-        <v>1915</v>
       </c>
       <c r="J263" s="7"/>
       <c r="K263" s="7"/>
@@ -20471,17 +20469,17 @@
       <c r="M263" s="7"/>
       <c r="N263" s="8"/>
       <c r="O263" s="5" t="s">
+        <v>1915</v>
+      </c>
+      <c r="P263" s="5" t="s">
         <v>1916</v>
-      </c>
-      <c r="P263" s="5" t="s">
-        <v>1917</v>
       </c>
       <c r="Q263" s="7"/>
       <c r="R263" s="7"/>
     </row>
     <row r="264" spans="1:18" ht="50.25" customHeight="1">
       <c r="A264" s="5" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B264" s="5" t="s">
         <v>1208</v>
@@ -20493,20 +20491,20 @@
         <v>26</v>
       </c>
       <c r="E264" s="5" t="s">
+        <v>1918</v>
+      </c>
+      <c r="F264" s="5" t="s">
         <v>1919</v>
-      </c>
-      <c r="F264" s="5" t="s">
-        <v>1920</v>
       </c>
       <c r="G264" s="5" t="str">
         <f t="shared" si="5"/>
         <v>farley2025liftvr</v>
       </c>
       <c r="H264" s="7" t="s">
+        <v>1920</v>
+      </c>
+      <c r="I264" s="7" t="s">
         <v>1921</v>
-      </c>
-      <c r="I264" s="7" t="s">
-        <v>1922</v>
       </c>
       <c r="J264" s="7"/>
       <c r="K264" s="7"/>
@@ -20514,17 +20512,17 @@
       <c r="M264" s="7"/>
       <c r="N264" s="8"/>
       <c r="O264" s="5" t="s">
+        <v>1922</v>
+      </c>
+      <c r="P264" s="5" t="s">
         <v>1923</v>
-      </c>
-      <c r="P264" s="5" t="s">
-        <v>1924</v>
       </c>
       <c r="Q264" s="7"/>
       <c r="R264" s="7"/>
     </row>
     <row r="265" spans="1:18" ht="50.25" customHeight="1">
       <c r="A265" s="5" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B265" s="5" t="s">
         <v>108</v>
@@ -20533,23 +20531,23 @@
         <v>45772</v>
       </c>
       <c r="D265" s="5" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="E265" s="5" t="s">
         <v>1839</v>
       </c>
       <c r="F265" s="5" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="G265" s="5" t="str">
         <f t="shared" si="5"/>
         <v>park2025exploring</v>
       </c>
       <c r="H265" s="7" t="s">
+        <v>1927</v>
+      </c>
+      <c r="I265" s="7" t="s">
         <v>1928</v>
-      </c>
-      <c r="I265" s="7" t="s">
-        <v>1929</v>
       </c>
       <c r="J265" s="7"/>
       <c r="K265" s="7"/>
@@ -20557,17 +20555,17 @@
       <c r="M265" s="7"/>
       <c r="N265" s="8"/>
       <c r="O265" s="5" t="s">
+        <v>1929</v>
+      </c>
+      <c r="P265" s="5" t="s">
         <v>1930</v>
-      </c>
-      <c r="P265" s="5" t="s">
-        <v>1931</v>
       </c>
       <c r="Q265" s="7"/>
       <c r="R265" s="7"/>
     </row>
     <row r="266" spans="1:18" ht="50.25" customHeight="1">
       <c r="A266" s="5" t="s">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B266" s="5" t="s">
         <v>108</v>
@@ -20582,17 +20580,17 @@
         <v>1497</v>
       </c>
       <c r="F266" s="21" t="s">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="G266" s="5" t="str">
         <f t="shared" si="5"/>
         <v>rigling2025reverse</v>
       </c>
       <c r="H266" s="7" t="s">
+        <v>1933</v>
+      </c>
+      <c r="I266" s="7" t="s">
         <v>1934</v>
-      </c>
-      <c r="I266" s="7" t="s">
-        <v>1935</v>
       </c>
       <c r="J266" s="7"/>
       <c r="K266" s="7"/>
@@ -20600,17 +20598,17 @@
       <c r="M266" s="7"/>
       <c r="N266" s="8"/>
       <c r="O266" s="5" t="s">
+        <v>1935</v>
+      </c>
+      <c r="P266" s="5" t="s">
         <v>1936</v>
-      </c>
-      <c r="P266" s="5" t="s">
-        <v>1937</v>
       </c>
       <c r="Q266" s="7"/>
       <c r="R266" s="7"/>
     </row>
     <row r="267" spans="1:18" ht="50.25" customHeight="1">
       <c r="A267" s="5" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B267" s="5" t="s">
         <v>108</v>
@@ -20625,37 +20623,37 @@
         <v>1620</v>
       </c>
       <c r="F267" s="5" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="G267" s="5" t="str">
         <f t="shared" si="5"/>
         <v>yang2025exploring</v>
       </c>
       <c r="H267" s="7" t="s">
+        <v>1939</v>
+      </c>
+      <c r="I267" s="7" t="s">
         <v>1940</v>
       </c>
-      <c r="I267" s="7" t="s">
+      <c r="J267" s="7" t="s">
         <v>1941</v>
-      </c>
-      <c r="J267" s="7" t="s">
-        <v>1942</v>
       </c>
       <c r="K267" s="7"/>
       <c r="L267" s="7"/>
       <c r="M267" s="7"/>
       <c r="N267" s="8"/>
       <c r="O267" s="5" t="s">
+        <v>1942</v>
+      </c>
+      <c r="P267" s="5" t="s">
         <v>1943</v>
-      </c>
-      <c r="P267" s="5" t="s">
-        <v>1944</v>
       </c>
       <c r="Q267" s="7"/>
       <c r="R267" s="7"/>
     </row>
     <row r="268" spans="1:18" ht="50.25" customHeight="1">
       <c r="A268" s="5" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>108</v>
@@ -20670,37 +20668,37 @@
         <v>1620</v>
       </c>
       <c r="F268" s="20" t="s">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="G268" s="5" t="str">
         <f t="shared" si="5"/>
         <v>yang2025who</v>
       </c>
       <c r="H268" s="7" t="s">
+        <v>1946</v>
+      </c>
+      <c r="I268" s="7" t="s">
         <v>1947</v>
       </c>
-      <c r="I268" s="7" t="s">
+      <c r="J268" s="7" t="s">
         <v>1948</v>
-      </c>
-      <c r="J268" s="7" t="s">
-        <v>1949</v>
       </c>
       <c r="K268" s="7"/>
       <c r="L268" s="7"/>
       <c r="M268" s="7"/>
       <c r="N268" s="8"/>
       <c r="O268" s="5" t="s">
+        <v>1949</v>
+      </c>
+      <c r="P268" s="5" t="s">
         <v>1950</v>
-      </c>
-      <c r="P268" s="5" t="s">
-        <v>1951</v>
       </c>
       <c r="Q268" s="7"/>
       <c r="R268" s="7"/>
     </row>
     <row r="269" spans="1:18" ht="50.25" customHeight="1">
       <c r="A269" s="5" t="s">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B269" s="5" t="s">
         <v>108</v>
@@ -20715,40 +20713,40 @@
         <v>363</v>
       </c>
       <c r="F269" s="5" t="s">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="G269" s="5" t="str">
         <f t="shared" si="5"/>
         <v>rau2025traversing</v>
       </c>
       <c r="H269" s="7" t="s">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="I269" s="7" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="J269" s="7" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="K269" s="7"/>
       <c r="L269" s="7"/>
       <c r="M269" s="7"/>
       <c r="N269" s="8"/>
       <c r="O269" s="5" t="s">
+        <v>1954</v>
+      </c>
+      <c r="P269" s="5" t="s">
         <v>1955</v>
-      </c>
-      <c r="P269" s="5" t="s">
-        <v>1956</v>
       </c>
       <c r="Q269" s="7"/>
       <c r="R269" s="7"/>
     </row>
     <row r="270" spans="1:18" ht="50.25" customHeight="1">
       <c r="A270" s="5" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B270" s="5" t="s">
         <v>1957</v>
-      </c>
-      <c r="B270" s="5" t="s">
-        <v>1958</v>
       </c>
       <c r="C270" s="6">
         <v>45736</v>
@@ -20757,17 +20755,17 @@
         <v>289</v>
       </c>
       <c r="E270" s="5" t="s">
+        <v>1958</v>
+      </c>
+      <c r="F270" s="5" t="s">
         <v>1959</v>
-      </c>
-      <c r="F270" s="5" t="s">
-        <v>1960</v>
       </c>
       <c r="G270" s="5" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E270," ",REPT(" ",100)),100)) &amp; YEAR(C270) &amp; IFERROR(LEFT(A270,FIND(" ",A270)-1),A270)), ":", "")</f>
         <v>zhou2025personal</v>
       </c>
       <c r="H270" s="7" t="s">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="I270" s="7"/>
       <c r="J270" s="7"/>
@@ -20776,20 +20774,20 @@
       <c r="M270" s="7"/>
       <c r="N270" s="8"/>
       <c r="O270" s="5" t="s">
+        <v>1961</v>
+      </c>
+      <c r="P270" s="23" t="s">
         <v>1962</v>
-      </c>
-      <c r="P270" s="23" t="s">
-        <v>1963</v>
       </c>
       <c r="Q270" s="7"/>
       <c r="R270" s="7"/>
     </row>
     <row r="271" spans="1:18" ht="50.25" customHeight="1">
       <c r="A271" s="5" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B271" s="5" t="s">
         <v>1967</v>
-      </c>
-      <c r="B271" s="5" t="s">
-        <v>1968</v>
       </c>
       <c r="C271" s="6">
         <v>45809</v>
@@ -20808,30 +20806,30 @@
         <v>park2025design</v>
       </c>
       <c r="H271" s="7" t="s">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="I271" s="7"/>
       <c r="J271" s="7" t="s">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="K271" s="7"/>
       <c r="L271" s="7"/>
       <c r="M271" s="7"/>
       <c r="N271" s="8" t="s">
+        <v>1970</v>
+      </c>
+      <c r="O271" s="5" t="s">
         <v>1971</v>
       </c>
-      <c r="O271" s="5" t="s">
+      <c r="P271" s="23" t="s">
         <v>1972</v>
-      </c>
-      <c r="P271" s="23" t="s">
-        <v>1973</v>
       </c>
       <c r="Q271" s="7"/>
       <c r="R271" s="7"/>
     </row>
     <row r="272" spans="1:18" ht="50.25" customHeight="1">
       <c r="A272" s="24" t="s">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B272" s="24" t="s">
         <v>1563</v>
@@ -20846,34 +20844,34 @@
         <v>1564</v>
       </c>
       <c r="F272" s="24" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="G272" s="24" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="H272" s="24"/>
       <c r="I272" s="24"/>
       <c r="J272" s="24"/>
       <c r="K272" s="26" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="L272" s="24"/>
       <c r="M272" s="24"/>
       <c r="N272" s="24" t="s">
+        <v>1976</v>
+      </c>
+      <c r="O272" s="29" t="s">
         <v>1977</v>
       </c>
-      <c r="O272" s="29" t="s">
-        <v>1978</v>
-      </c>
       <c r="P272" s="28" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="Q272" s="27"/>
       <c r="R272" s="27"/>
     </row>
     <row r="273" spans="1:18" ht="50.25" customHeight="1">
       <c r="A273" s="5" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>127</v>
@@ -20888,14 +20886,14 @@
         <v>1698</v>
       </c>
       <c r="F273" s="5" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="G273" s="5" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E273," ",REPT(" ",100)),100)) &amp; YEAR(C273) &amp; IFERROR(LEFT(A273,FIND(" ",A273)-1),A273)), ":", "")</f>
         <v>bauer2025voronoi</v>
       </c>
       <c r="H273" s="18" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="I273" s="7"/>
       <c r="J273" s="7"/>
@@ -20903,17 +20901,17 @@
       <c r="L273" s="7"/>
       <c r="M273" s="7"/>
       <c r="N273" s="8" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="O273" s="5" t="s">
+        <v>1981</v>
+      </c>
+      <c r="P273" s="23" t="s">
         <v>1982</v>
-      </c>
-      <c r="P273" s="23" t="s">
-        <v>1983</v>
       </c>
       <c r="Q273" s="7"/>
       <c r="R273" s="7" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
     </row>
   </sheetData>
@@ -21668,15 +21666,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bcc6a80-9cbb-4ef4-81b1-0de6e4d1e31e">
@@ -21685,6 +21674,15 @@
     <TaxCatchAll xmlns="2f19b678-e8b7-409b-86f9-6b59659c2b24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21707,14 +21705,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74FA3D6-0E8A-4136-B53D-83DD582CB2C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -21723,4 +21713,12 @@
     <ds:schemaRef ds:uri="2f19b678-e8b7-409b-86f9-6b59659c2b24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adds all missing bibtex and links where possible
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krautecn\Documents\GitHub\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19659FF-6B2C-45D7-B75B-85858637CEB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0DB6B4-66B4-4F85-9940-11BDEE48DE63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2451" uniqueCount="1988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2471" uniqueCount="2008">
   <si>
     <t>Title</t>
   </si>
@@ -9101,6 +9101,149 @@
    &lt;img style="width: 20px; height: 20px; vertical-align: middle;" alt="stamp icon" src="../assets/img/misc/stamp.png"&gt;
     Graphics Replicability Stamp
 &lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>IEEE Dataport</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Information Visualization</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1260/147807709788549402</t>
+  </si>
+  <si>
+    <t>https://www.ixpug.org/images/docs/IXPUG_Annual_Spring_Conference_2018/intel_ixpug_spring_2018_sdvis_megamol.pdf</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1109/ISMAR-Adjunct60411.2023.00028</t>
+  </si>
+  <si>
+    <t>https://virtual.ieeevis.org/year/2023/poster_v-vis-posters-1080.html</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/profile/Tessa-Talsma/publication/384967034_Towards_a_common_understanding_of_Simulator_Sickness/links/6717977168ac304149aa5ca2/Towards-a-common-understanding-of-Simulator-Sickness.pdf</t>
+  </si>
+  <si>
+    <t>The Old Library of Trinity College Dublin, built in 1732, is an internationally renowned research library. In recent decades it has also become a major tourist attraction in Dublin, with the display of the Book of Kells within the Old Library now drawing over half a million visitors per year. The Preservation and Conservation Department of the Library has raised concerns about the impact of the environment on the collection. The location of the building in the city centre, large visitor numbers, and the conditions within the  building are putting the collection at risk. In developing a strategic plan to find solutions to these problems, the department has been assessing and documenting the current situation. This paper introduces ongoing work on a system to visualise the collected data, which includes: dust levels and dispersion, internal and external temperature and relative humidity levels, and visitor numbers in the Old Library. We are developing a user interface for which the data, originally stored in various file formats, is consolidated in a database which can be explored using a 3D virtual reconstruction of the Old Library. With this novel technique, it is also possible to compare and assess the relationships between the various datasets in context.</t>
+  </si>
+  <si>
+    <t>Modern automobiles come with a high degree of electronicand an enormous amount of in-car communication activi-ties. This leads to an increasing complexity which challengesautomotive engineers in detecting and analyzing erroneouscommunication processes. In this contribution we presentresults of our studies on current working behaviour and envi-ronments of analysis and diagnosis experts in the automotiveindustry. While we found a sufficient hardware and softwaresupport in single user environments, co-located collabora-tive environments are characterized by multiple hardwaredevices but by a lack of specific software to support collabo-rating in these multiple display environment (MDEs). Aftera detailed user analysis and evaluation we derive system re-quirements for this new MDE application area and discussits challenges.</t>
+  </si>
+  <si>
+    <t>This document represents a practical summary from experiences and results gained during the research project “VALiD - Visual Analytics in Data-Driven Journalism”. It addresses some of the major issues around data journalism practice. A large part is taken from a review of the research literature review on this topic. You can find the references for this review and links to other project-related resources at the end of this document. This document addresses journalists and communicators who have little to no experience in the field of data-intensive newswork.</t>
+  </si>
+  <si>
+    <t>@inproceedings{sedlmair2008requirements,
+  title={Requirements for a mde system to support collaborative in-car communication diagnostics},
+  author={Sedlmair, Michael and Baur, Dominikus and Boring, Sebastian and Isenberg, Petra and Jurmu, Marko and Butz, Andreas},
+  booktitle={CSCW Workshop on Beyond the Laboratory: Supporting Authentic Collaboration with Multiple Displays},
+  year={2008}
+}</t>
+  </si>
+  <si>
+    <t>@article{doi:10.1260/147807709788549402,
+	title        = {LibViz: Data Visualisation of the Old Library},
+	author       = {K. Ruhland and C. O'Sullivan and S. Bioletti and M. Sedlmair},
+	year         = 2009,
+	journal      = {International Journal of Architectural Computing},
+	volume       = 7,
+	number       = 1,
+	pages        = {177--192},
+	doi          = {10.1260/147807709788549402},
+	url          = {https://doi.org/10.1260/147807709788549402},
+	eprint       = {https://doi.org/10.1260/147807709788549402},
+	abstract     = {The Old Library of Trinity College Dublin, built in 1732, is an internationally renowned research library. In recent decades it has also become a major tourist attraction in Dublin, with the display of the Book of Kells within the Old Library now drawing over half a million visitors per year. The Preservation and Conservation Department of the Library has raised concerns about the impact of the environment on the collection. The location of the building in the city centre, large visitor numbers, and the conditions within the building are putting the collection at risk. In developing a strategic plan to find solutions to these problems, the department has been assessing and documenting the current situation. This paper introduces ongoing work on a system to visualise the collected data, which includes: dust levels and dispersion, internal and external temperature and relative humidity levels, and visitor numbers in the Old Library. We are developing a user interface for which the data, originally stored in various file formats, is consolidated in a database which can be explored using a 3D virtual reconstruction of the Old Library. With this novel technique, it is also possible to compare and assess the relationships between the various datasets in context.}
+}</t>
+  </si>
+  <si>
+    <t>@misc{Busdaten,
+  title        = {Visualisierung von Busdaten – Fehleranalyse im Forschungsprojekt AutobahnVis},
+  journal      = {Journal of Automobil Elektronik},
+  author       = {Michael Sedlmair and Michael Schraut and Wolfgang Hintermaier},
+  url = {https://www.all-electronics.de/automotive-transportation/visualisierung-von-busdaten.html},
+  year         = 2011,
+mont = {10},
+abstrac = {Wie können Methoden der Informationsvisualisierung die explorative Analyse von Busdaten verbessern? Ein Forschungsprojekt mit dem Namen „AutobahnVis“ zeigt beispielhaft, wie Visualisierung neue Einsichten in komplexe Zusammenhänge ermöglicht und zur Fehleranalyse von Busaufzeichnungen beiträgt.}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{hube2016virtual,
+	title        = {Virtual UNREALity: Exploring Alternative Visualization Techniques for Virtual Reality},
+	author       = {Natalie Hube, Hannes Grusla, Mathias Müller, Ingmar S. Franke, Tobias Günther, Rainer Groh},
+	year         = 2016,
+	month        = {07},
+	series       = {xCoAX},
+	url          = {http://2016.xcoax.org/pdf/xcoax2016-Hube.pdf},
+	abstract     = {Virtual Reality (VR) offers new ways to perceive and interact with virtual content. Apart from photo-realism, VR can be used to explore new ways of visualization and interaction. In this contribution, we describe two student projects, which focused on creating innovative concepts for an artistic VR experience. We provide a review of sources of inspiration ranging from standard NPR-techniques through movies, interactive artworks and games to phenomena of human perception. Based on this wide collection of material we describe the prototypes, and discuss observations during implementation and from user feedback. Finally, possible future directions to use the potential of VR as a tool for novel, artful and unconventional experiences are discussed.}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{zoomPB,
+	title        = {A Zoomable Product Browser for Elastic Displays},
+	author       = {Mathias Müller and Mandy Keck and Thomas Gründer and Natalie Hube and Rainer Groh},
+	year         = 2017,
+	booktitle    = {Proceedings xCoAx 2017},
+	publisher    = {5th Conference on Computation, Communication, Aesthetics &amp; X},
+	address      = {Lisbon, Portugal},
+	pages        = 10,
+	url          = {http://2017.xcoax.org/pdf/xcoax2017-Muller.pdf},
+	date         = {2017-07-05},
+	abstract     = {In this paper, we present an interaction and visualization concept for elastic displays. The interaction concept was inspired by the search process of a rummage table to explore a large set of product data. The basic approach uses a similarity-based search pattern – based on a small set of items, the user refines the search result by examining similar items and exchanging them with items from the current result. A physically-based approach is used to interact with the data by deforming the surface of the elastic display. The presented visualization concept uses glyphs to directly compare items at a glance. Zoomable UI techniques controlled by the deformation of the elastic surface allow to display different levels of detail for each item.},
+	keywords     = {Glyphs, Interface Design},
+	pubstate     = {published},
+	tppubtype    = {conference}
+}</t>
+  </si>
+  <si>
+    <t>@misc{aigner2018valid,
+	title        = {Data Journalism - Guidelines and Best Practices for Getting Started},
+	author       = {Wolfgang Aigner, Eva Goldgruber, Florian Grassinger, Robert Gutounig, Alexander Rind, Michael Sedlmair, Christina Stoiber},
+	year         = 2018,
+	url          = {https://github.com/VALIDproject/ddj-booklet},
+	howpublished = {\url{https://www.nasa.gov/nh/pluto-the-other-red-planet}},
+	mont         = {01},
+	abstract     = {This document represents a practical summary from experiences and results gained during the research project “VALiD - Visual Analytics in Data-Driven Journalism”. It addresses some of the major issues around data journalism practice. A large part is taken from a review of the research literature review on this topic. You can find the references for this review and links to other project-related resources at the end of this document. This document addresses journalists and communicators who have little to no experience in the field of data-intensive newswork.}
+}</t>
+  </si>
+  <si>
+    <t>@misc{aigner2018valid,
+	title        = {The Data in Your Hands: Exploring Novel Interaction Techniques and Data Visualization Approaches for Immersive Data Analytics},
+	author       = {Natalie Hube, Mathias Müller},
+	year         = 2018,
+	url = {http://ceur-ws.org/Vol-2108/paper2.pdf},
+	mont         = {05},
+	abstract     = {In this paper, we describe a concept for visualization and interaction with a large data set in an virtual environment. The core idea uses the traditional flat 2D representation as a base visualization but lets the user transform it into a spatial 3D visualizations on demand. Our visualization and interaction concept targets data analysts to use it for exploration and analysis, utilizing virtual reality to gain insight into complex data sets. The concept is based on the use of Parallel Sets for the representation of categorical data. By extending the conventional 2D Parallel Sets with a third dimension, correlations between path variables and the related number of items belonging to a specific node can be visualized. Furthermore, the concept uses virtual reality controllers in combination with a head-mounted display to control additional views. The purpose of the paper is to describe the core concepts and challenges for this type of spatial visualization and the related interaction design, including the use of gestures for direct manuipulation and a hand-attached menu for complex actions			}
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'@inproceedings{zhang20233d,
+	title        = {3D Hapkit: A Low-Cost, Open-Source, 3-DOF Haptic Device Based on the Delta Parallel Mechanism},
+	author       = {Han Zhang, Jan Ulrich Bartels, Jeremy Brown},
+	year         = 2017,
+	url = {https://2023.worldhaptics.org/wp-content/uploads/2023/06/1070-doc.pdf},
+	mont         = {07},
+	abstract     = {We present our work on an open-source, low-cost, 3-Degree Of Freedom (3-DOF) haptic device for use in haptic education. The device is based on three open-source 1-DOF haptic devices in a delta configuration and can be produced using commonly available rapid prototyping methodologies such as 3D printing and laser cutting. We also demonstrate a simple interaction with a virtual environment.}
+}
+</t>
+  </si>
+  <si>
+    <t>@misc{fan2023virtual,
+      title={irtual Reality Training for Nosocomial Infections Prevention}, 
+      author={Mengjie Fan, Shaoxing Zhang, Xintian Zhao, Xingyao Yu, Liang Zhou},
+      year={2023},
+      mont={10},
+      eprint={2312.11144},
+      url={Nosocomial infections (or healthcare-associated infections) can greatly affect public health. The prevention and control of nosocomial infections rely on effective training of medical personnel on the correct use of personal prevention equipment (PPE). We introduce a virtual reality (VR) method that simulates the real environment of a hospital and supports repeated immersive practice of PPE donning and doffing. A VR prototype is created and receives positive feedback from a domain expert. The effectiveness of our method will be evaluated in a comparative user study.}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{talsma2024towards,
+author = {Talsma, Tessa and de Winkel, Ksander and Happee, Riender},
+year = {2024},
+month = {09},
+pages = {},
+title = {Towards a common understanding of Simulator Sickness}
+}</t>
   </si>
 </sst>
 </file>
@@ -9217,11 +9360,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -9298,12 +9442,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
+    <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -9385,6 +9534,34 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -9730,8 +9907,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P258" workbookViewId="0">
-      <selection activeCell="Q262" sqref="Q262"/>
+    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q273" sqref="Q273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
@@ -9832,13 +10010,21 @@
       <c r="G2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="7"/>
+      <c r="H2" s="31" t="s">
+        <v>1990</v>
+      </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="8"/>
+      <c r="O2" s="5" t="s">
+        <v>1995</v>
+      </c>
+      <c r="P2" s="23" t="s">
+        <v>1999</v>
+      </c>
       <c r="Q2" s="5" t="s">
         <v>23</v>
       </c>
@@ -9873,6 +10059,12 @@
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="8"/>
+      <c r="O3" s="5" t="s">
+        <v>1996</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>1998</v>
+      </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
     </row>
@@ -10401,6 +10593,9 @@
       <c r="O17" s="5" t="s">
         <v>125</v>
       </c>
+      <c r="P17" s="23" t="s">
+        <v>2000</v>
+      </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
@@ -11334,6 +11529,9 @@
       <c r="O41" s="5" t="s">
         <v>302</v>
       </c>
+      <c r="P41" s="23" t="s">
+        <v>2001</v>
+      </c>
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
     </row>
@@ -11665,7 +11863,9 @@
         <v>rau2017challenges</v>
       </c>
       <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
+      <c r="I50" s="7" t="s">
+        <v>1991</v>
+      </c>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
@@ -11734,7 +11934,7 @@
       <c r="G52" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="H52" s="7" t="s">
+      <c r="H52" s="31" t="s">
         <v>378</v>
       </c>
       <c r="I52" s="7"/>
@@ -11981,7 +12181,7 @@
       <c r="O58" s="5" t="s">
         <v>422</v>
       </c>
-      <c r="P58" s="5" t="s">
+      <c r="P58" s="23" t="s">
         <v>423</v>
       </c>
       <c r="Q58" s="7"/>
@@ -12063,6 +12263,9 @@
       <c r="O60" s="5" t="s">
         <v>433</v>
       </c>
+      <c r="P60" s="23" t="s">
+        <v>2002</v>
+      </c>
       <c r="Q60" s="7"/>
       <c r="R60" s="7"/>
     </row>
@@ -12404,6 +12607,12 @@
         <v>494</v>
       </c>
       <c r="N69" s="8"/>
+      <c r="O69" s="5" t="s">
+        <v>1997</v>
+      </c>
+      <c r="P69" s="23" t="s">
+        <v>2003</v>
+      </c>
       <c r="Q69" s="7"/>
       <c r="R69" s="7"/>
     </row>
@@ -12684,6 +12893,9 @@
       <c r="O76" s="5" t="s">
         <v>538</v>
       </c>
+      <c r="P76" s="23" t="s">
+        <v>2004</v>
+      </c>
       <c r="Q76" s="7"/>
       <c r="R76" s="7"/>
     </row>
@@ -15549,6 +15761,9 @@
       <c r="A148" s="5" t="s">
         <v>1038</v>
       </c>
+      <c r="B148" s="5" t="s">
+        <v>1988</v>
+      </c>
       <c r="C148" s="6">
         <v>44336</v>
       </c>
@@ -18430,6 +18645,9 @@
       <c r="O215" s="5" t="s">
         <v>1561</v>
       </c>
+      <c r="P215" s="23" t="s">
+        <v>2005</v>
+      </c>
       <c r="Q215" s="7"/>
       <c r="R215" s="7"/>
     </row>
@@ -18848,7 +19066,9 @@
         <f t="shared" si="4"/>
         <v>sayara2023designing</v>
       </c>
-      <c r="H225" s="7"/>
+      <c r="H225" s="7" t="s">
+        <v>1992</v>
+      </c>
       <c r="I225" s="7" t="s">
         <v>1637</v>
       </c>
@@ -18971,7 +19191,9 @@
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E228," ",REPT(" ",100)),100)) &amp; YEAR(C228) &amp; IFERROR(LEFT(A228,FIND(" ",A228)-1),A228)), ":", "")</f>
         <v>fan2023virtual</v>
       </c>
-      <c r="H228" s="7"/>
+      <c r="H228" s="7" t="s">
+        <v>1993</v>
+      </c>
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
       <c r="K228" s="7"/>
@@ -18981,6 +19203,9 @@
       <c r="O228" s="5" t="s">
         <v>1657</v>
       </c>
+      <c r="P228" s="23" t="s">
+        <v>2006</v>
+      </c>
       <c r="Q228" s="7"/>
       <c r="R228" s="7"/>
     </row>
@@ -19231,7 +19456,7 @@
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E234," ",REPT(" ",100)),100)) &amp; YEAR(C234) &amp; IFERROR(LEFT(A234,FIND(" ",A234)-1),A234)), ":", "")</f>
         <v>bauer2023visual</v>
       </c>
-      <c r="H234" t="s">
+      <c r="H234" s="30" t="s">
         <v>1700</v>
       </c>
       <c r="I234" s="7" t="s">
@@ -19256,6 +19481,9 @@
     <row r="235" spans="1:18" ht="50.25" customHeight="1">
       <c r="A235" s="5" t="s">
         <v>1705</v>
+      </c>
+      <c r="B235" s="5" t="s">
+        <v>1989</v>
       </c>
       <c r="C235" s="6">
         <v>45292</v>
@@ -19958,13 +20186,18 @@
       </c>
       <c r="H251" s="7"/>
       <c r="I251" s="7"/>
-      <c r="J251" s="7"/>
+      <c r="J251" s="31" t="s">
+        <v>1994</v>
+      </c>
       <c r="K251" s="7"/>
       <c r="L251" s="7"/>
       <c r="M251" s="7"/>
       <c r="N251" s="8"/>
       <c r="O251" s="5" t="s">
         <v>1828</v>
+      </c>
+      <c r="P251" s="23" t="s">
+        <v>2007</v>
       </c>
       <c r="Q251" s="7"/>
       <c r="R251" s="7"/>
@@ -20915,6 +21148,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O2:R273">
+    <cfRule type="expression" dxfId="21" priority="1">
+      <formula>ISBLANK(O2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H127" r:id="rId1" xr:uid="{CEE39E7F-917B-4159-B668-437B94191ED7}"/>
     <hyperlink ref="J136" r:id="rId2" xr:uid="{4C56950B-D68B-414F-BCA0-02A053D8DA28}"/>
@@ -21401,11 +21639,14 @@
     <hyperlink ref="J271" r:id="rId483" xr:uid="{E9215BA0-45A1-4652-AEF1-A00C1295EFDA}"/>
     <hyperlink ref="K272" r:id="rId484" xr:uid="{23479075-357B-4E14-B7E5-34B750AE71BA}"/>
     <hyperlink ref="H273" r:id="rId485" xr:uid="{1FE003AB-2EE7-4EEB-9167-234FAA90E3FA}"/>
+    <hyperlink ref="H234" r:id="rId486" xr:uid="{D00D3DA6-793E-4BDC-B559-793669F9EA45}"/>
+    <hyperlink ref="H2" r:id="rId487" xr:uid="{D805A780-3AAA-4440-9FDD-C1C372AD1E3B}"/>
+    <hyperlink ref="J251" r:id="rId488" xr:uid="{287A9795-26B3-4739-AD9F-1A3CA2B25B68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId486"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId489"/>
   <tableParts count="1">
-    <tablePart r:id="rId487"/>
+    <tablePart r:id="rId490"/>
   </tableParts>
 </worksheet>
 </file>
@@ -21666,6 +21907,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9bcc6a80-9cbb-4ef4-81b1-0de6e4d1e31e">
@@ -21674,15 +21924,6 @@
     <TaxCatchAll xmlns="2f19b678-e8b7-409b-86f9-6b59659c2b24" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -21705,6 +21946,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E74FA3D6-0E8A-4136-B53D-83DD582CB2C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -21713,12 +21962,4 @@
     <ds:schemaRef ds:uri="2f19b678-e8b7-409b-86f9-6b59659c2b24"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E6D51A-19DE-4C35-92E0-270E15734A61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removes empty urls from bibtex
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krautecn\Documents\GitHub\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0DB6B4-66B4-4F85-9940-11BDEE48DE63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C8B4F0-06DB-4678-BBAC-165049762420}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9057,16 +9057,6 @@
     <t>krieglstein2025a</t>
   </si>
   <si>
-    <t>@inproceedings{krieglstein2025hybrid,
-author = {Krieglstein, Jan and Kolberg, Jan and Sousa Calepso, Aimée and Kraus, Werner and Sedlmair, Michael},
-title = {A Hybrid User Interface Combining AR, Desktop, and Mobile Interfaces for Enhanced Industrial Robot Programming},
-year = {2025},
-publisher = {IEEE},
-doi = {},
-booktitle = {International Conference on Automation and Robotics},
-}</t>
-  </si>
-  <si>
     <t>Voronoi Cell Interface-Based Parameter Sensitivity Analysis for Labeled Samples</t>
   </si>
   <si>
@@ -9243,6 +9233,15 @@
 month = {09},
 pages = {},
 title = {Towards a common understanding of Simulator Sickness}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{krieglstein2025hybrid,
+author = {Krieglstein, Jan and Kolberg, Jan and Sousa Calepso, Aimée and Kraus, Werner and Sedlmair, Michael},
+title = {A Hybrid User Interface Combining AR, Desktop, and Mobile Interfaces for Enhanced Industrial Robot Programming},
+year = {2025},
+publisher = {IEEE},
+booktitle = {International Conference on Automation and Robotics},
 }</t>
   </si>
 </sst>
@@ -9452,7 +9451,7 @@
     <cellStyle name="Link" xfId="2" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="21">
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -9534,27 +9533,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -9907,9 +9885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q273" sqref="Q273"/>
+    <sheetView tabSelected="1" topLeftCell="H112" workbookViewId="0">
+      <selection activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1"/>
@@ -10011,7 +9988,7 @@
         <v>22</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -10020,10 +9997,10 @@
       <c r="M2" s="7"/>
       <c r="N2" s="8"/>
       <c r="O2" s="5" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="P2" s="23" t="s">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>23</v>
@@ -10060,10 +10037,10 @@
       <c r="M3" s="7"/>
       <c r="N3" s="8"/>
       <c r="O3" s="5" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
@@ -10594,7 +10571,7 @@
         <v>125</v>
       </c>
       <c r="P17" s="23" t="s">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
@@ -11530,7 +11507,7 @@
         <v>302</v>
       </c>
       <c r="P41" s="23" t="s">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="Q41" s="7"/>
       <c r="R41" s="7"/>
@@ -11864,7 +11841,7 @@
       </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
@@ -12264,7 +12241,7 @@
         <v>433</v>
       </c>
       <c r="P60" s="23" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="Q60" s="7"/>
       <c r="R60" s="7"/>
@@ -12608,10 +12585,10 @@
       </c>
       <c r="N69" s="8"/>
       <c r="O69" s="5" t="s">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="P69" s="23" t="s">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="Q69" s="7"/>
       <c r="R69" s="7"/>
@@ -12894,7 +12871,7 @@
         <v>538</v>
       </c>
       <c r="P76" s="23" t="s">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="Q76" s="7"/>
       <c r="R76" s="7"/>
@@ -15762,7 +15739,7 @@
         <v>1038</v>
       </c>
       <c r="B148" s="5" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="C148" s="6">
         <v>44336</v>
@@ -18646,7 +18623,7 @@
         <v>1561</v>
       </c>
       <c r="P215" s="23" t="s">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="Q215" s="7"/>
       <c r="R215" s="7"/>
@@ -19067,7 +19044,7 @@
         <v>sayara2023designing</v>
       </c>
       <c r="H225" s="7" t="s">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="I225" s="7" t="s">
         <v>1637</v>
@@ -19192,7 +19169,7 @@
         <v>fan2023virtual</v>
       </c>
       <c r="H228" s="7" t="s">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="I228" s="7"/>
       <c r="J228" s="7"/>
@@ -19204,7 +19181,7 @@
         <v>1657</v>
       </c>
       <c r="P228" s="23" t="s">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="Q228" s="7"/>
       <c r="R228" s="7"/>
@@ -19483,7 +19460,7 @@
         <v>1705</v>
       </c>
       <c r="B235" s="5" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="C235" s="6">
         <v>45292</v>
@@ -20187,7 +20164,7 @@
       <c r="H251" s="7"/>
       <c r="I251" s="7"/>
       <c r="J251" s="31" t="s">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="K251" s="7"/>
       <c r="L251" s="7"/>
@@ -20197,7 +20174,7 @@
         <v>1828</v>
       </c>
       <c r="P251" s="23" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="Q251" s="7"/>
       <c r="R251" s="7"/>
@@ -20663,7 +20640,7 @@
         <v>1909</v>
       </c>
       <c r="Q262" s="7" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="R262" s="7"/>
     </row>
@@ -21097,14 +21074,14 @@
         <v>1977</v>
       </c>
       <c r="P272" s="28" t="s">
-        <v>1979</v>
+        <v>2007</v>
       </c>
       <c r="Q272" s="27"/>
       <c r="R272" s="27"/>
     </row>
     <row r="273" spans="1:18" ht="50.25" customHeight="1">
       <c r="A273" s="5" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>127</v>
@@ -21119,14 +21096,14 @@
         <v>1698</v>
       </c>
       <c r="F273" s="5" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="G273" s="5" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E273," ",REPT(" ",100)),100)) &amp; YEAR(C273) &amp; IFERROR(LEFT(A273,FIND(" ",A273)-1),A273)), ":", "")</f>
         <v>bauer2025voronoi</v>
       </c>
       <c r="H273" s="18" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="I273" s="7"/>
       <c r="J273" s="7"/>
@@ -21134,22 +21111,22 @@
       <c r="L273" s="7"/>
       <c r="M273" s="7"/>
       <c r="N273" s="8" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="O273" s="5" t="s">
+        <v>1980</v>
+      </c>
+      <c r="P273" s="23" t="s">
         <v>1981</v>
-      </c>
-      <c r="P273" s="23" t="s">
-        <v>1982</v>
       </c>
       <c r="Q273" s="7"/>
       <c r="R273" s="7" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O2:R273">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>ISBLANK(O2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixes some more stuff in bib
</commit_message>
<xml_diff>
--- a/Papers.xlsx
+++ b/Papers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krautecn\Documents\GitHub\visvar.github.io\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\GitHub\visvar.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76D07BF-FEAA-4ABE-8C32-44C19E236061}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019F1538-E38F-4DC2-9AF7-DC3E5102FCEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1500" windowWidth="28800" windowHeight="15216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Public" sheetId="1" r:id="rId1"/>
@@ -6626,16 +6626,6 @@
 }</t>
   </si>
   <si>
-    <t>@article{eirich2021vis,
-	author = {Joscha Eirich and Jakob Bonart and Dominik J{\"a}ckle and Michael Sedlmair and Ute Schmid and Kai Fischbach and Tobias Schreck and J{\"u}rgen Bernard},
-	title = {{IRVINE}: A Design Study on Analyzing Correlation Patterns of Electrical Engines},
-	journal = {IEEE Trans. Visualization and Computer Graphics (TVCG, Proc. VIS 2021)},
-	note = {To appear. Best paper award},
-  	doi = {https://doi.org/10.1109/TVCG.2021.3114797},
-	year = {2021}
-}</t>
-  </si>
-  <si>
     <t>@article{10.1145/3488546,
 author = {Smiley, Jim and Lee, Benjamin and Tandon, Siddhant and Cordeil, Maxime and Besan\c{c}on, Lonni and Knibbe, Jarrod and Jenny, Bernhard and Dwyer, Tim},
 title = {The MADE-Axis: A Modular Actuated Device to Embody the Axis of a Data Dimension},
@@ -7305,15 +7295,6 @@
 }</t>
   </si>
   <si>
-    <t>@misc{fan2023virtual,
-      title={irtual Reality Training for Nosocomial Infections Prevention}, 
-      author={Mengjie Fan, Shaoxing Zhang, Xintian Zhao, Xingyao Yu, Liang Zhou},
-      year={2023},
-      mont={10},
-      url={Nosocomial infections (or healthcare-associated infections) can greatly affect public health. The prevention and control of nosocomial infections rely on effective training of medical personnel on the correct use of personal prevention equipment (PPE). We introduce a virtual reality (VR) method that simulates the real environment of a hospital and supports repeated immersive practice of PPE donning and doffing. A VR prototype is created and receives positive feedback from a domain expert. The effectiveness of our method will be evaluated in a comparative user study.}
-}</t>
-  </si>
-  <si>
     <t>Christian Berhold, Daniel Herrscher, Sebastian Boring, Andreas Butz</t>
   </si>
   <si>
@@ -7849,26 +7830,6 @@
 }</t>
   </si>
   <si>
-    <t>@inproceedings{krauter2021don,
-	title        = {Don't Catch It: An Interactive Virtual-Reality Environment to Learn About COVID-19 Measures Using Gamification Elements},
-	shorttitle   = {Don't Catch It},
-	author       = {Krauter\textasteriskcentered, Christian and Vogelsang\textasteriskcentered, Jonas and Sousa Calepso, Aim{\'e}e and Angerbauer, Katrin and Sedlmair, Michael},
-	year         = {2021},
-	month        = {9},
-	booktitle    = {Proc. Mensch Und Computer},
-	publisher    = {ACM},
-	series       = {MuC},
-	pages        = {593--596},
-	doi          = {10.1145/3473856.3474031},
-	isbn         = {978-1-4503-8645-6},
-	abstract     = {The world is still under the influence of the COVID-19 pandemic. Even though vaccines are deployed as rapidly as possible, it is still necessary to use other measures to reduce the spread of the virus. Measures such as social distancing or wearing a mask receive a lot of criticism. Therefore, we want to demonstrate a serious game to help the players understand these measures better and show them why they are still necessary. The player of the game has to avoid other agents to keep their risk of a COVID-19 infection low. The game uses Virtual Reality through a Head-Mounted-Display to deliver an immersive and enjoyable experience. Gamification elements are used to engage the user with the game while they explore various environments. We also implemented visualizations that help the user with social distancing. \textasteriskcentered Both authors contributed equally to this research.},
-	bibtex_show  = {true},
-	preview      = {krauter2021Don\_teaser.png},
-	pdf          = {krauter2021Don.pdf},
-	video        = {https://www.doi.org/10.1145/3473856.3474031}
-}</t>
-  </si>
-  <si>
     <t>@article{MachicaoNMLB21,
 	title        = {A visual analysis method of randomness for classifying and ranking pseudo-random number generators},
 	author       = {Jeaneth Machicao and Quynh Quang Ngo and Vladimir Molchanov and Lars Linsen and Odemir M. Bruno},
@@ -7955,24 +7916,6 @@
 }</t>
   </si>
   <si>
-    <t>@inproceedings{rzayev2019notification,
-	title        = {Notification in VR: The Effect of Notification Placement, Task and Environment},
-	shorttitle   = {Notification in VR},
-	author       = {Rzayev, Rufat and Mayer, Sven and Krauter, Christian and Henze, Niels},
-	year         = {2019},
-	month        = {10},
-	booktitle    = {Proc. Symp. Computer-Human Interaction in Play},
-	publisher    = {ACM},
-	series       = {CHI Play},
-	pages        = {199--211},
-	doi          = {10.1145/3311350.3347190},
-	isbn         = {978-1-4503-6688-5},
-	bibtex_show  = {true},
-	abstract     = {Virtual reality (VR) is commonly used for entertainment applications but is also increasingly employed for a large number of use cases such as digital prototyping or training workers. Here, VR is key to present an immersive secondary world. VR enables experiences that are close to reality, regardless of time and place. However, highly immersive VR can result in missing digital information from the real world, such as important notifications. For efficient notification presentation in VR, it is necessary to understand how notifications should be integrated in VR without breaking the immersion. Thus, we conducted a study with 24 participants to investigate notification placement in VR while playing games, learning, and solving problems. We compared placing notifications using a Head-Up Display, On-Body, Floating, and In-Situ in open, semi-open, and closed VR environments. We found significant effects of notification placement and task on how notifications are perceived in VR. Insights from our study inform the design of VR applications that support digital notifications.},
-	video        = {http://doi.org/10.1145/3311350.3347190}
-}</t>
-  </si>
-  <si>
     <t>@inproceedings{NgoHL17,
 	title        = {Visual Analytics of Global Parameters in Simulation Ensembles of ODE-based Excitable Network Dynamics},
 	author       = {Quynh Quang Ngo and Marc{-}Thorsten H{\"{u}}tt and Lars Linsen},
@@ -8688,6 +8631,56 @@
 	year          = {2008},
 	journal       = {Electronic Communications of the EASST},
 	volume        = {13}
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{krauter2021don,
+	title        = {Don't Catch It: An Interactive Virtual-Reality Environment to Learn About COVID-19 Measures Using Gamification Elements},
+	shorttitle   = {Don't Catch It},
+	author       = {Krauter, Christian and Vogelsang, Jonas and Sousa Calepso, Aim{\'e}e and Angerbauer, Katrin and Sedlmair, Michael},
+	year         = {2021},
+	month        = {9},
+	booktitle    = {Proc. Mensch Und Computer},
+	publisher    = {ACM},
+	series       = {MuC},
+	pages        = {593--596},
+	doi          = {10.1145/3473856.3474031},
+	isbn         = {978-1-4503-8645-6},
+	abstract     = {The world is still under the influence of the COVID-19 pandemic. Even though vaccines are deployed as rapidly as possible, it is still necessary to use other measures to reduce the spread of the virus. Measures such as social distancing or wearing a mask receive a lot of criticism. Therefore, we want to demonstrate a serious game to help the players understand these measures better and show them why they are still necessary. The player of the game has to avoid other agents to keep their risk of a COVID-19 infection low. The game uses Virtual Reality through a Head-Mounted-Display to deliver an immersive and enjoyable experience. Gamification elements are used to engage the user with the game while they explore various environments. We also implemented visualizations that help the user with social distancing. \textasteriskcentered Both authors contributed equally to this research.},
+}</t>
+  </si>
+  <si>
+    <t>@inproceedings{rzayev2019notification,
+	title        = {Notification in VR: The Effect of Notification Placement, Task and Environment},
+	shorttitle   = {Notification in VR},
+	author       = {Rzayev, Rufat and Mayer, Sven and Krauter, Christian and Henze, Niels},
+	year         = {2019},
+	month        = {10},
+	booktitle    = {Proc. Symp. Computer-Human Interaction in Play},
+	publisher    = {ACM},
+	series       = {CHI Play},
+	pages        = {199--211},
+	doi          = {10.1145/3311350.3347190},
+	isbn         = {978-1-4503-6688-5},
+	abstract     = {Virtual reality (VR) is commonly used for entertainment applications but is also increasingly employed for a large number of use cases such as digital prototyping or training workers. Here, VR is key to present an immersive secondary world. VR enables experiences that are close to reality, regardless of time and place. However, highly immersive VR can result in missing digital information from the real world, such as important notifications. For efficient notification presentation in VR, it is necessary to understand how notifications should be integrated in VR without breaking the immersion. Thus, we conducted a study with 24 participants to investigate notification placement in VR while playing games, learning, and solving problems. We compared placing notifications using a Head-Up Display, On-Body, Floating, and In-Situ in open, semi-open, and closed VR environments. We found significant effects of notification placement and task on how notifications are perceived in VR. Insights from our study inform the design of VR applications that support digital notifications.},
+}</t>
+  </si>
+  <si>
+    <t>@misc{fan2023virtual,
+      title={Virtual Reality Training for Nosocomial Infections Prevention}, 
+      author={Mengjie Fan, Shaoxing Zhang, Xintian Zhao, Xingyao Yu, Liang Zhou},
+      year={2023},
+      month={10},
+      url={Nosocomial infections (or healthcare-associated infections) can greatly affect public health. The prevention and control of nosocomial infections rely on effective training of medical personnel on the correct use of personal prevention equipment (PPE). We introduce a virtual reality (VR) method that simulates the real environment of a hospital and supports repeated immersive practice of PPE donning and doffing. A VR prototype is created and receives positive feedback from a domain expert. The effectiveness of our method will be evaluated in a comparative user study.}
+}</t>
+  </si>
+  <si>
+    <t>@article{eirich2021vis,
+	author = {Joscha Eirich and Jakob Bonart and Dominik J{\"a}ckle and Michael Sedlmair and Ute Schmid and Kai Fischbach and Tobias Schreck and J{\"u}rgen Bernard},
+	title = {{IRVINE}: A Design Study on Analyzing Correlation Patterns of Electrical Engines},
+	journal = {IEEE Trans. Visualization and Computer Graphics (TVCG, Proc. VIS 2021)},
+  	doi = {https://doi.org/10.1109/TVCG.2021.3114797},
+	year = {2021}
 }</t>
   </si>
 </sst>
@@ -8808,9 +8801,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="33">
@@ -8876,7 +8868,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -8894,14 +8886,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-000B-0000-0000-000008000000}"/>
-    <cellStyle name="Link" xfId="2" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
     <dxf>
@@ -9234,7 +9225,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -9532,34 +9523,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R273"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P3" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="P155" workbookViewId="0">
+      <selection activeCell="P158" sqref="P158"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="50.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="60.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="99.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="38.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="99.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="46.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="67.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="68.28515625" style="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="255.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="208.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="4"/>
+    <col min="12" max="12" width="46.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="67.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="68.33203125" style="20" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="255.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="208.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="30.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9615,7 +9606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>18</v>
       </c>
@@ -9641,13 +9632,13 @@
         <v>1707</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="Q2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -9676,7 +9667,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>30</v>
       </c>
@@ -9702,10 +9693,10 @@
         <v>34</v>
       </c>
       <c r="P4" s="21" t="s">
-        <v>1927</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>35</v>
       </c>
@@ -9734,7 +9725,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -9760,7 +9751,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>47</v>
       </c>
@@ -9786,10 +9777,10 @@
         <v>52</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>1830</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>53</v>
       </c>
@@ -9818,10 +9809,10 @@
         <v>58</v>
       </c>
       <c r="P8" s="21" t="s">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>59</v>
       </c>
@@ -9835,7 +9826,7 @@
         <v>27</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>60</v>
@@ -9850,7 +9841,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>64</v>
       </c>
@@ -9876,10 +9867,10 @@
         <v>70</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>1900</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>71</v>
       </c>
@@ -9905,10 +9896,10 @@
         <v>76</v>
       </c>
       <c r="P11" s="22" t="s">
-        <v>1901</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>77</v>
       </c>
@@ -9943,7 +9934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>83</v>
       </c>
@@ -9969,10 +9960,10 @@
         <v>88</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>1908</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>89</v>
       </c>
@@ -10004,7 +9995,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>97</v>
       </c>
@@ -10033,7 +10024,7 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>103</v>
       </c>
@@ -10062,7 +10053,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>109</v>
       </c>
@@ -10088,10 +10079,10 @@
         <v>114</v>
       </c>
       <c r="P17" s="22" t="s">
-        <v>1832</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>115</v>
       </c>
@@ -10123,7 +10114,7 @@
         <v>1713</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>122</v>
       </c>
@@ -10155,7 +10146,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>129</v>
       </c>
@@ -10190,7 +10181,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>137</v>
       </c>
@@ -10222,7 +10213,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>144</v>
       </c>
@@ -10257,7 +10248,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>151</v>
       </c>
@@ -10286,7 +10277,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>158</v>
       </c>
@@ -10318,7 +10309,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>166</v>
       </c>
@@ -10350,7 +10341,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
         <v>173</v>
       </c>
@@ -10382,7 +10373,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>180</v>
       </c>
@@ -10411,10 +10402,10 @@
         <v>185</v>
       </c>
       <c r="P27" s="22" t="s">
-        <v>1885</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1881</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>186</v>
       </c>
@@ -10443,7 +10434,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>193</v>
       </c>
@@ -10472,7 +10463,7 @@
         <v>1729</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
         <v>198</v>
       </c>
@@ -10504,7 +10495,7 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>204</v>
       </c>
@@ -10536,7 +10527,7 @@
         <v>1714</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>211</v>
       </c>
@@ -10565,10 +10556,10 @@
         <v>218</v>
       </c>
       <c r="P32" s="21" t="s">
-        <v>1884</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1880</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>219</v>
       </c>
@@ -10597,7 +10588,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>224</v>
       </c>
@@ -10623,10 +10614,10 @@
         <v>230</v>
       </c>
       <c r="P34" s="21" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>231</v>
       </c>
@@ -10655,7 +10646,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>239</v>
       </c>
@@ -10681,10 +10672,10 @@
         <v>245</v>
       </c>
       <c r="P36" s="21" t="s">
-        <v>1899</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1895</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>246</v>
       </c>
@@ -10713,7 +10704,7 @@
         <v>1731</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>253</v>
       </c>
@@ -10742,7 +10733,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>260</v>
       </c>
@@ -10771,7 +10762,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>266</v>
       </c>
@@ -10804,10 +10795,10 @@
         <v>272</v>
       </c>
       <c r="P40" s="21" t="s">
-        <v>1883</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1879</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>273</v>
       </c>
@@ -10840,10 +10831,10 @@
         <v>278</v>
       </c>
       <c r="P41" s="22" t="s">
-        <v>1892</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>279</v>
       </c>
@@ -10872,7 +10863,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>286</v>
       </c>
@@ -10904,7 +10895,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>292</v>
       </c>
@@ -10940,7 +10931,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>301</v>
       </c>
@@ -10972,7 +10963,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>308</v>
       </c>
@@ -10998,10 +10989,10 @@
         <v>313</v>
       </c>
       <c r="P46" s="21" t="s">
-        <v>1897</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1893</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>314</v>
       </c>
@@ -11030,7 +11021,7 @@
         <v>1732</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>319</v>
       </c>
@@ -11059,7 +11050,7 @@
         <v>1733</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
         <v>326</v>
       </c>
@@ -11086,10 +11077,10 @@
         <v>331</v>
       </c>
       <c r="P49" s="22" t="s">
-        <v>1882</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>332</v>
       </c>
@@ -11119,7 +11110,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>338</v>
       </c>
@@ -11145,7 +11136,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>345</v>
       </c>
@@ -11174,7 +11165,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>352</v>
       </c>
@@ -11207,7 +11198,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>360</v>
       </c>
@@ -11230,10 +11221,10 @@
         <v>365</v>
       </c>
       <c r="P54" s="21" t="s">
-        <v>1898</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1894</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>366</v>
       </c>
@@ -11268,7 +11259,7 @@
         <v>1734</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>372</v>
       </c>
@@ -11297,7 +11288,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>379</v>
       </c>
@@ -11323,10 +11314,10 @@
         <v>383</v>
       </c>
       <c r="P57" s="22" t="s">
-        <v>1823</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>384</v>
       </c>
@@ -11359,10 +11350,10 @@
         <v>388</v>
       </c>
       <c r="P58" s="21" t="s">
-        <v>1875</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1871</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>389</v>
       </c>
@@ -11392,10 +11383,10 @@
         <v>392</v>
       </c>
       <c r="P59" s="22" t="s">
-        <v>1868</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>393</v>
       </c>
@@ -11425,10 +11416,10 @@
         <v>397</v>
       </c>
       <c r="P60" s="21" t="s">
-        <v>1881</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>398</v>
       </c>
@@ -11457,7 +11448,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>404</v>
       </c>
@@ -11486,7 +11477,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
         <v>410</v>
       </c>
@@ -11515,7 +11506,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
         <v>416</v>
       </c>
@@ -11544,7 +11535,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="24" t="s">
         <v>423</v>
       </c>
@@ -11577,10 +11568,10 @@
         <v>429</v>
       </c>
       <c r="P65" s="22" t="s">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>430</v>
       </c>
@@ -11609,7 +11600,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>436</v>
       </c>
@@ -11641,7 +11632,7 @@
         <v>1736</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
         <v>442</v>
       </c>
@@ -11667,10 +11658,10 @@
         <v>447</v>
       </c>
       <c r="P68" s="21" t="s">
-        <v>1824</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
         <v>448</v>
       </c>
@@ -11702,10 +11693,10 @@
         <v>1709</v>
       </c>
       <c r="P69" s="22" t="s">
-        <v>1880</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
         <v>456</v>
       </c>
@@ -11734,7 +11725,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
         <v>464</v>
       </c>
@@ -11763,7 +11754,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
         <v>469</v>
       </c>
@@ -11792,7 +11783,7 @@
         <v>1737</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
         <v>474</v>
       </c>
@@ -11831,7 +11822,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
         <v>480</v>
       </c>
@@ -11867,7 +11858,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
         <v>487</v>
       </c>
@@ -11900,7 +11891,7 @@
         <v>1739</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
         <v>492</v>
       </c>
@@ -11930,10 +11921,10 @@
         <v>495</v>
       </c>
       <c r="P76" s="21" t="s">
-        <v>1879</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
         <v>496</v>
       </c>
@@ -11963,7 +11954,7 @@
         <v>1740</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="7" t="s">
         <v>502</v>
       </c>
@@ -11998,7 +11989,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="7" t="s">
         <v>509</v>
       </c>
@@ -12030,10 +12021,10 @@
         <v>514</v>
       </c>
       <c r="P79" s="22" t="s">
-        <v>1877</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1873</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="7" t="s">
         <v>515</v>
       </c>
@@ -12062,10 +12053,10 @@
         <v>521</v>
       </c>
       <c r="P80" s="21" t="s">
-        <v>1878</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1874</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="7" t="s">
         <v>522</v>
       </c>
@@ -12098,7 +12089,7 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="7" t="s">
         <v>527</v>
       </c>
@@ -12127,7 +12118,7 @@
         <v>1716</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="7" t="s">
         <v>532</v>
       </c>
@@ -12153,10 +12144,10 @@
         <v>536</v>
       </c>
       <c r="P83" s="22" t="s">
-        <v>1825</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="7" t="s">
         <v>537</v>
       </c>
@@ -12186,10 +12177,10 @@
         <v>543</v>
       </c>
       <c r="P84" s="21" t="s">
-        <v>1902</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1898</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="7" t="s">
         <v>544</v>
       </c>
@@ -12218,7 +12209,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="7" t="s">
         <v>550</v>
       </c>
@@ -12247,7 +12238,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>556</v>
       </c>
@@ -12280,7 +12271,7 @@
         <v>1742</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>562</v>
       </c>
@@ -12309,10 +12300,10 @@
         <v>567</v>
       </c>
       <c r="P88" s="21" t="s">
-        <v>1907</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
         <v>568</v>
       </c>
@@ -12345,7 +12336,7 @@
         <v>1743</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="7" t="s">
         <v>573</v>
       </c>
@@ -12374,7 +12365,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="7" t="s">
         <v>581</v>
       </c>
@@ -12400,10 +12391,10 @@
         <v>585</v>
       </c>
       <c r="P91" s="22" t="s">
-        <v>1874</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1870</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="7" t="s">
         <v>586</v>
       </c>
@@ -12439,10 +12430,10 @@
         <v>592</v>
       </c>
       <c r="P92" s="21" t="s">
-        <v>1876</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1872</v>
+      </c>
+    </row>
+    <row r="93" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="7" t="s">
         <v>593</v>
       </c>
@@ -12456,7 +12447,7 @@
         <v>595</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="G93" s="7" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E93," ",REPT(" ",100)),100)) &amp; YEAR(C93) &amp; IFERROR(LEFT(A93,FIND(" ",A93)-1),A93)), ":", "")</f>
@@ -12469,10 +12460,10 @@
         <v>597</v>
       </c>
       <c r="P93" s="22" t="s">
-        <v>1873</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1869</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="24" t="s">
         <v>598</v>
       </c>
@@ -12505,7 +12496,7 @@
         <v>1744</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="7" t="s">
         <v>604</v>
       </c>
@@ -12534,7 +12525,7 @@
         <v>1745</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="7" t="s">
         <v>611</v>
       </c>
@@ -12563,7 +12554,7 @@
         <v>1746</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="7" t="s">
         <v>617</v>
       </c>
@@ -12605,7 +12596,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="7" t="s">
         <v>623</v>
       </c>
@@ -12635,10 +12626,10 @@
         <v>627</v>
       </c>
       <c r="P98" s="21" t="s">
-        <v>1872</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1868</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="7" t="s">
         <v>628</v>
       </c>
@@ -12671,10 +12662,10 @@
         <v>633</v>
       </c>
       <c r="P99" s="22" t="s">
-        <v>1871</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1867</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="7" t="s">
         <v>634</v>
       </c>
@@ -12700,10 +12691,10 @@
         <v>639</v>
       </c>
       <c r="P100" s="21" t="s">
-        <v>1926</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1922</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="7" t="s">
         <v>640</v>
       </c>
@@ -12726,16 +12717,16 @@
         <v>644</v>
       </c>
       <c r="J101" s="32" t="s">
-        <v>1925</v>
+        <v>1921</v>
       </c>
       <c r="O101" s="7" t="s">
         <v>645</v>
       </c>
       <c r="P101" s="22" t="s">
-        <v>1924</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="7" t="s">
         <v>646</v>
       </c>
@@ -12764,10 +12755,10 @@
         <v>651</v>
       </c>
       <c r="P102" s="21" t="s">
-        <v>1870</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="7" t="s">
         <v>652</v>
       </c>
@@ -12796,10 +12787,10 @@
         <v>657</v>
       </c>
       <c r="P103" s="22" t="s">
-        <v>1869</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1865</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="7" t="s">
         <v>658</v>
       </c>
@@ -12831,10 +12822,10 @@
         <v>664</v>
       </c>
       <c r="P104" s="21" t="s">
-        <v>1896</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="7" t="s">
         <v>665</v>
       </c>
@@ -12864,10 +12855,10 @@
         <v>668</v>
       </c>
       <c r="P105" s="22" t="s">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1914</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="7" t="s">
         <v>669</v>
       </c>
@@ -12900,10 +12891,10 @@
         <v>675</v>
       </c>
       <c r="P106" s="21" t="s">
-        <v>1867</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
         <v>676</v>
       </c>
@@ -12930,10 +12921,10 @@
         <v>681</v>
       </c>
       <c r="P107" s="22" t="s">
-        <v>1923</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1919</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
         <v>682</v>
       </c>
@@ -12963,10 +12954,10 @@
         <v>688</v>
       </c>
       <c r="P108" s="21" t="s">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="7" t="s">
         <v>689</v>
       </c>
@@ -12996,10 +12987,10 @@
         <v>693</v>
       </c>
       <c r="P109" s="22" t="s">
-        <v>1917</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1913</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="7" t="s">
         <v>694</v>
       </c>
@@ -13028,10 +13019,10 @@
         <v>699</v>
       </c>
       <c r="P110" s="21" t="s">
-        <v>1906</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="7" t="s">
         <v>700</v>
       </c>
@@ -13063,7 +13054,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="7" t="s">
         <v>706</v>
       </c>
@@ -13089,10 +13080,10 @@
         <v>710</v>
       </c>
       <c r="P112" s="21" t="s">
-        <v>1866</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1863</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="7" t="s">
         <v>711</v>
       </c>
@@ -13121,7 +13112,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="7" t="s">
         <v>717</v>
       </c>
@@ -13154,10 +13145,10 @@
         <v>723</v>
       </c>
       <c r="P114" s="21" t="s">
-        <v>1916</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="7" t="s">
         <v>724</v>
       </c>
@@ -13183,10 +13174,10 @@
         <v>730</v>
       </c>
       <c r="P115" s="22" t="s">
-        <v>1865</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1862</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
         <v>731</v>
       </c>
@@ -13215,10 +13206,10 @@
         <v>736</v>
       </c>
       <c r="P116" s="21" t="s">
-        <v>1915</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="24" t="s">
         <v>737</v>
       </c>
@@ -13247,10 +13238,10 @@
         <v>742</v>
       </c>
       <c r="P117" s="22" t="s">
-        <v>1905</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1901</v>
+      </c>
+    </row>
+    <row r="118" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>743</v>
       </c>
@@ -13286,7 +13277,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="7" t="s">
         <v>749</v>
       </c>
@@ -13315,7 +13306,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="7" t="s">
         <v>756</v>
       </c>
@@ -13344,7 +13335,7 @@
         <v>1750</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="7" t="s">
         <v>762</v>
       </c>
@@ -13376,7 +13367,7 @@
         <v>1751</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="7" t="s">
         <v>769</v>
       </c>
@@ -13405,7 +13396,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="7" t="s">
         <v>776</v>
       </c>
@@ -13443,7 +13434,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="7" t="s">
         <v>783</v>
       </c>
@@ -13476,10 +13467,10 @@
         <v>789</v>
       </c>
       <c r="P124" s="21" t="s">
-        <v>1864</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1861</v>
+      </c>
+    </row>
+    <row r="125" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="7" t="s">
         <v>790</v>
       </c>
@@ -13512,7 +13503,7 @@
         <v>1752</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="7" t="s">
         <v>795</v>
       </c>
@@ -13554,7 +13545,7 @@
         <v>1753</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="7" t="s">
         <v>802</v>
       </c>
@@ -13590,10 +13581,10 @@
         <v>808</v>
       </c>
       <c r="P127" s="22" t="s">
-        <v>1863</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1860</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="7" t="s">
         <v>809</v>
       </c>
@@ -13623,10 +13614,10 @@
         <v>812</v>
       </c>
       <c r="P128" s="21" t="s">
-        <v>1862</v>
-      </c>
-    </row>
-    <row r="129" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="129" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="7" t="s">
         <v>813</v>
       </c>
@@ -13655,7 +13646,7 @@
         <v>1754</v>
       </c>
     </row>
-    <row r="130" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="7" t="s">
         <v>819</v>
       </c>
@@ -13684,7 +13675,7 @@
         <v>1755</v>
       </c>
     </row>
-    <row r="131" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="7" t="s">
         <v>825</v>
       </c>
@@ -13720,7 +13711,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="132" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="7" t="s">
         <v>831</v>
       </c>
@@ -13752,7 +13743,7 @@
         <v>1757</v>
       </c>
     </row>
-    <row r="133" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="7" t="s">
         <v>837</v>
       </c>
@@ -13788,7 +13779,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="134" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="7" t="s">
         <v>843</v>
       </c>
@@ -13820,7 +13811,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="135" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="7" t="s">
         <v>851</v>
       </c>
@@ -13865,7 +13856,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="136" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="7" t="s">
         <v>859</v>
       </c>
@@ -13898,7 +13889,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="137" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="7" t="s">
         <v>863</v>
       </c>
@@ -13931,7 +13922,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="138" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="24" t="s">
         <v>869</v>
       </c>
@@ -13964,7 +13955,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="139" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="7" t="s">
         <v>874</v>
       </c>
@@ -13993,7 +13984,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="140" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="7" t="s">
         <v>881</v>
       </c>
@@ -14019,10 +14010,10 @@
         <v>885</v>
       </c>
       <c r="P140" s="21" t="s">
-        <v>1835</v>
-      </c>
-    </row>
-    <row r="141" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="141" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="7" t="s">
         <v>886</v>
       </c>
@@ -14048,10 +14039,10 @@
         <v>890</v>
       </c>
       <c r="P141" s="22" t="s">
-        <v>1836</v>
-      </c>
-    </row>
-    <row r="142" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="7" t="s">
         <v>891</v>
       </c>
@@ -14083,7 +14074,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="7" t="s">
         <v>897</v>
       </c>
@@ -14115,7 +14106,7 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="144" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="7" t="s">
         <v>903</v>
       </c>
@@ -14145,10 +14136,10 @@
         <v>908</v>
       </c>
       <c r="P144" s="21" t="s">
-        <v>1861</v>
-      </c>
-    </row>
-    <row r="145" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="7" t="s">
         <v>909</v>
       </c>
@@ -14181,7 +14172,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="7" t="s">
         <v>913</v>
       </c>
@@ -14210,10 +14201,10 @@
         <v>919</v>
       </c>
       <c r="P146" s="21" t="s">
-        <v>1904</v>
-      </c>
-    </row>
-    <row r="147" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1900</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="7" t="s">
         <v>920</v>
       </c>
@@ -14245,10 +14236,10 @@
         <v>927</v>
       </c>
       <c r="P147" s="22" t="s">
-        <v>1895</v>
-      </c>
-    </row>
-    <row r="148" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1891</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="7" t="s">
         <v>928</v>
       </c>
@@ -14280,10 +14271,10 @@
         <v>934</v>
       </c>
       <c r="P148" s="21" t="s">
-        <v>1903</v>
-      </c>
-    </row>
-    <row r="149" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1899</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="7" t="s">
         <v>935</v>
       </c>
@@ -14315,7 +14306,7 @@
         <v>1763</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="7" t="s">
         <v>940</v>
       </c>
@@ -14348,7 +14339,7 @@
         <v>1764</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="7" t="s">
         <v>947</v>
       </c>
@@ -14380,7 +14371,7 @@
         <v>1765</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="7" t="s">
         <v>953</v>
       </c>
@@ -14419,10 +14410,10 @@
         <v>960</v>
       </c>
       <c r="P152" s="21" t="s">
-        <v>1894</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="7" t="s">
         <v>961</v>
       </c>
@@ -14451,10 +14442,10 @@
         <v>968</v>
       </c>
       <c r="P153" s="22" t="s">
-        <v>1860</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1924</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="7" t="s">
         <v>969</v>
       </c>
@@ -14483,10 +14474,10 @@
         <v>974</v>
       </c>
       <c r="P154" s="21" t="s">
-        <v>1914</v>
-      </c>
-    </row>
-    <row r="155" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1910</v>
+      </c>
+    </row>
+    <row r="155" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="7" t="s">
         <v>975</v>
       </c>
@@ -14530,7 +14521,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="7" t="s">
         <v>984</v>
       </c>
@@ -14566,7 +14557,7 @@
         <v>1767</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="7" t="s">
         <v>990</v>
       </c>
@@ -14592,10 +14583,10 @@
         <v>996</v>
       </c>
       <c r="P157" s="22" t="s">
-        <v>1859</v>
-      </c>
-    </row>
-    <row r="158" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="7" t="s">
         <v>997</v>
       </c>
@@ -14624,13 +14615,13 @@
         <v>1002</v>
       </c>
       <c r="P158" s="21" t="s">
-        <v>1768</v>
+        <v>1927</v>
       </c>
       <c r="Q158" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="7" t="s">
         <v>1003</v>
       </c>
@@ -14659,10 +14650,10 @@
         <v>1008</v>
       </c>
       <c r="P159" s="22" t="s">
-        <v>1913</v>
-      </c>
-    </row>
-    <row r="160" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1909</v>
+      </c>
+    </row>
+    <row r="160" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="7" t="s">
         <v>1009</v>
       </c>
@@ -14694,10 +14685,10 @@
         <v>1015</v>
       </c>
       <c r="P160" s="21" t="s">
-        <v>1893</v>
-      </c>
-    </row>
-    <row r="161" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1889</v>
+      </c>
+    </row>
+    <row r="161" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="7" t="s">
         <v>1016</v>
       </c>
@@ -14738,7 +14729,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="162" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="7" t="s">
         <v>1026</v>
       </c>
@@ -14767,10 +14758,10 @@
         <v>1030</v>
       </c>
       <c r="P162" s="21" t="s">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="163" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1887</v>
+      </c>
+    </row>
+    <row r="163" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="7" t="s">
         <v>1031</v>
       </c>
@@ -14784,7 +14775,7 @@
         <v>1032</v>
       </c>
       <c r="F163" s="7" t="s">
-        <v>1920</v>
+        <v>1916</v>
       </c>
       <c r="G163" s="7" t="s">
         <v>1033</v>
@@ -14802,13 +14793,13 @@
         <v>1037</v>
       </c>
       <c r="P163" s="22" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="Q163" s="7" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="164" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="7" t="s">
         <v>1038</v>
       </c>
@@ -14843,7 +14834,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="165" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="7" t="s">
         <v>1048</v>
       </c>
@@ -14876,7 +14867,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="166" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="27" t="s">
         <v>1056</v>
       </c>
@@ -14909,7 +14900,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="167" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="7" t="s">
         <v>1063</v>
       </c>
@@ -14942,10 +14933,10 @@
         <v>1067</v>
       </c>
       <c r="P167" s="22" t="s">
-        <v>1922</v>
-      </c>
-    </row>
-    <row r="168" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="168" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="7" t="s">
         <v>1068</v>
       </c>
@@ -14981,7 +14972,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="169" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="7" t="s">
         <v>1075</v>
       </c>
@@ -15011,7 +15002,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="170" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="7" t="s">
         <v>1082</v>
       </c>
@@ -15053,10 +15044,10 @@
         <v>1091</v>
       </c>
       <c r="P170" s="21" t="s">
-        <v>1770</v>
-      </c>
-    </row>
-    <row r="171" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="171" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="7" t="s">
         <v>1092</v>
       </c>
@@ -15089,10 +15080,10 @@
         <v>1096</v>
       </c>
       <c r="P171" s="22" t="s">
-        <v>1771</v>
-      </c>
-    </row>
-    <row r="172" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1770</v>
+      </c>
+    </row>
+    <row r="172" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="7" t="s">
         <v>1097</v>
       </c>
@@ -15128,10 +15119,10 @@
         <v>1102</v>
       </c>
       <c r="P172" s="21" t="s">
-        <v>1772</v>
-      </c>
-    </row>
-    <row r="173" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1771</v>
+      </c>
+    </row>
+    <row r="173" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="7" t="s">
         <v>1103</v>
       </c>
@@ -15163,13 +15154,13 @@
         <v>1109</v>
       </c>
       <c r="P173" s="22" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="Q173" s="7" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="174" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="7" t="s">
         <v>1110</v>
       </c>
@@ -15199,10 +15190,10 @@
         <v>1115</v>
       </c>
       <c r="P174" s="21" t="s">
-        <v>1774</v>
-      </c>
-    </row>
-    <row r="175" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1773</v>
+      </c>
+    </row>
+    <row r="175" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="7" t="s">
         <v>1116</v>
       </c>
@@ -15238,12 +15229,12 @@
         <v>1122</v>
       </c>
       <c r="P175" s="22" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="Q175" s="7"/>
       <c r="R175" s="7"/>
     </row>
-    <row r="176" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="7" t="s">
         <v>1123</v>
       </c>
@@ -15279,12 +15270,12 @@
         <v>1127</v>
       </c>
       <c r="P176" s="21" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="Q176" s="7"/>
       <c r="R176" s="7"/>
     </row>
-    <row r="177" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="7" t="s">
         <v>1128</v>
       </c>
@@ -15314,10 +15305,10 @@
         <v>1131</v>
       </c>
       <c r="P177" s="22" t="s">
-        <v>1777</v>
-      </c>
-    </row>
-    <row r="178" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="178" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="7" t="s">
         <v>1132</v>
       </c>
@@ -15353,10 +15344,10 @@
         <v>1138</v>
       </c>
       <c r="P178" s="21" t="s">
-        <v>1778</v>
-      </c>
-    </row>
-    <row r="179" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="179" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="7" t="s">
         <v>1139</v>
       </c>
@@ -15386,11 +15377,11 @@
         <v>1144</v>
       </c>
       <c r="P179" s="22" t="s">
-        <v>1858</v>
+        <v>1856</v>
       </c>
       <c r="R179" s="7"/>
     </row>
-    <row r="180" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="7" t="s">
         <v>1145</v>
       </c>
@@ -15426,13 +15417,13 @@
         <v>1151</v>
       </c>
       <c r="P180" s="21" t="s">
-        <v>1912</v>
+        <v>1908</v>
       </c>
       <c r="R180" s="7" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="181" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="7" t="s">
         <v>1153</v>
       </c>
@@ -15461,11 +15452,11 @@
         <v>1159</v>
       </c>
       <c r="P181" s="22" t="s">
-        <v>1837</v>
+        <v>1835</v>
       </c>
       <c r="R181" s="7"/>
     </row>
-    <row r="182" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="7" t="s">
         <v>1160</v>
       </c>
@@ -15507,7 +15498,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="183" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="7" t="s">
         <v>1167</v>
       </c>
@@ -15533,10 +15524,10 @@
         <v>1171</v>
       </c>
       <c r="P183" s="22" t="s">
-        <v>1857</v>
-      </c>
-    </row>
-    <row r="184" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="184" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="7" t="s">
         <v>1172</v>
       </c>
@@ -15566,10 +15557,10 @@
         <v>1177</v>
       </c>
       <c r="P184" s="21" t="s">
-        <v>1779</v>
-      </c>
-    </row>
-    <row r="185" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="185" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="7" t="s">
         <v>1178</v>
       </c>
@@ -15599,11 +15590,11 @@
         <v>1183</v>
       </c>
       <c r="P185" s="22" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="R185" s="7"/>
     </row>
-    <row r="186" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="7" t="s">
         <v>1184</v>
       </c>
@@ -15633,10 +15624,10 @@
         <v>1187</v>
       </c>
       <c r="P186" s="21" t="s">
-        <v>1856</v>
-      </c>
-    </row>
-    <row r="187" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="187" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="7" t="s">
         <v>1188</v>
       </c>
@@ -15666,10 +15657,10 @@
         <v>1193</v>
       </c>
       <c r="P187" s="22" t="s">
-        <v>1781</v>
-      </c>
-    </row>
-    <row r="188" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="188" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="7" t="s">
         <v>1194</v>
       </c>
@@ -15705,10 +15696,10 @@
         <v>1198</v>
       </c>
       <c r="P188" s="21" t="s">
-        <v>1782</v>
-      </c>
-    </row>
-    <row r="189" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="189" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="7" t="s">
         <v>1199</v>
       </c>
@@ -15738,10 +15729,10 @@
         <v>1202</v>
       </c>
       <c r="P189" s="22" t="s">
-        <v>1783</v>
-      </c>
-    </row>
-    <row r="190" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="190" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="7" t="s">
         <v>1203</v>
       </c>
@@ -15777,10 +15768,10 @@
         <v>1209</v>
       </c>
       <c r="P190" s="21" t="s">
-        <v>1784</v>
-      </c>
-    </row>
-    <row r="191" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="191" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="7" t="s">
         <v>1210</v>
       </c>
@@ -15813,10 +15804,10 @@
         <v>1216</v>
       </c>
       <c r="P191" s="22" t="s">
-        <v>1785</v>
-      </c>
-    </row>
-    <row r="192" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="192" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="7" t="s">
         <v>1217</v>
       </c>
@@ -15845,10 +15836,10 @@
         <v>1223</v>
       </c>
       <c r="P192" s="21" t="s">
-        <v>1855</v>
-      </c>
-    </row>
-    <row r="193" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="7" t="s">
         <v>1224</v>
       </c>
@@ -15881,10 +15872,10 @@
         <v>1227</v>
       </c>
       <c r="P193" s="22" t="s">
-        <v>1786</v>
-      </c>
-    </row>
-    <row r="194" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="7" t="s">
         <v>1228</v>
       </c>
@@ -15917,7 +15908,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="195" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="7" t="s">
         <v>1236</v>
       </c>
@@ -15951,10 +15942,10 @@
         <v>1241</v>
       </c>
       <c r="P195" s="22" t="s">
-        <v>1787</v>
-      </c>
-    </row>
-    <row r="196" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>1242</v>
       </c>
@@ -15986,10 +15977,10 @@
         <v>1249</v>
       </c>
       <c r="P196" s="21" t="s">
-        <v>1788</v>
-      </c>
-    </row>
-    <row r="197" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>1250</v>
       </c>
@@ -16027,13 +16018,13 @@
         <v>1258</v>
       </c>
       <c r="P197" s="22" t="s">
-        <v>1854</v>
+        <v>1852</v>
       </c>
       <c r="Q197" s="7" t="s">
         <v>1259</v>
       </c>
     </row>
-    <row r="198" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>1260</v>
       </c>
@@ -16071,7 +16062,7 @@
         <v>1268</v>
       </c>
     </row>
-    <row r="199" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>1269</v>
       </c>
@@ -16107,7 +16098,7 @@
         <v>1272</v>
       </c>
     </row>
-    <row r="200" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>1273</v>
       </c>
@@ -16140,10 +16131,10 @@
         <v>1279</v>
       </c>
       <c r="P200" s="21" t="s">
-        <v>1789</v>
-      </c>
-    </row>
-    <row r="201" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
         <v>1280</v>
       </c>
@@ -16176,7 +16167,7 @@
         <v>1285</v>
       </c>
     </row>
-    <row r="202" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="7" t="s">
         <v>1286</v>
       </c>
@@ -16209,7 +16200,7 @@
         <v>1292</v>
       </c>
     </row>
-    <row r="203" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="7" t="s">
         <v>1293</v>
       </c>
@@ -16239,7 +16230,7 @@
         <v>1299</v>
       </c>
     </row>
-    <row r="204" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="7" t="s">
         <v>1300</v>
       </c>
@@ -16269,10 +16260,10 @@
         <v>1306</v>
       </c>
       <c r="P204" s="21" t="s">
-        <v>1911</v>
-      </c>
-    </row>
-    <row r="205" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1907</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
         <v>1307</v>
       </c>
@@ -16298,10 +16289,10 @@
         <v>1313</v>
       </c>
       <c r="P205" s="22" t="s">
-        <v>1853</v>
-      </c>
-    </row>
-    <row r="206" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="7" t="s">
         <v>1314</v>
       </c>
@@ -16337,7 +16328,7 @@
       </c>
       <c r="Q206" s="7"/>
     </row>
-    <row r="207" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="7" t="s">
         <v>1320</v>
       </c>
@@ -16378,7 +16369,7 @@
         <v>1722</v>
       </c>
     </row>
-    <row r="208" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="7" t="s">
         <v>1329</v>
       </c>
@@ -16413,7 +16404,7 @@
         <v>1723</v>
       </c>
     </row>
-    <row r="209" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="7" t="s">
         <v>1336</v>
       </c>
@@ -16452,7 +16443,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="210" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="7" t="s">
         <v>1342</v>
       </c>
@@ -16482,7 +16473,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="211" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="7" t="s">
         <v>1347</v>
       </c>
@@ -16518,7 +16509,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="212" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="7" t="s">
         <v>1353</v>
       </c>
@@ -16551,10 +16542,10 @@
         <v>1356</v>
       </c>
       <c r="P212" s="21" t="s">
-        <v>1850</v>
-      </c>
-    </row>
-    <row r="213" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="7" t="s">
         <v>1357</v>
       </c>
@@ -16586,10 +16577,10 @@
         <v>1361</v>
       </c>
       <c r="P213" s="22" t="s">
-        <v>1851</v>
-      </c>
-    </row>
-    <row r="214" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="7" t="s">
         <v>1362</v>
       </c>
@@ -16622,10 +16613,10 @@
         <v>1365</v>
       </c>
       <c r="P214" s="21" t="s">
-        <v>1852</v>
-      </c>
-    </row>
-    <row r="215" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="7" t="s">
         <v>1366</v>
       </c>
@@ -16652,10 +16643,10 @@
         <v>1371</v>
       </c>
       <c r="P215" s="22" t="s">
-        <v>1890</v>
-      </c>
-    </row>
-    <row r="216" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="7" t="s">
         <v>1372</v>
       </c>
@@ -16688,7 +16679,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="217" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="7" t="s">
         <v>1379</v>
       </c>
@@ -16718,10 +16709,10 @@
         <v>1384</v>
       </c>
       <c r="P217" s="22" t="s">
-        <v>1790</v>
-      </c>
-    </row>
-    <row r="218" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="7" t="s">
         <v>1385</v>
       </c>
@@ -16754,11 +16745,11 @@
         <v>1390</v>
       </c>
       <c r="P218" s="21" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="Q218" s="7"/>
     </row>
-    <row r="219" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="7" t="s">
         <v>1391</v>
       </c>
@@ -16787,10 +16778,10 @@
         <v>1396</v>
       </c>
       <c r="P219" s="22" t="s">
-        <v>1792</v>
-      </c>
-    </row>
-    <row r="220" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="7" t="s">
         <v>1397</v>
       </c>
@@ -16823,10 +16814,10 @@
         <v>1403</v>
       </c>
       <c r="P220" s="21" t="s">
-        <v>1819</v>
-      </c>
-    </row>
-    <row r="221" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="7" t="s">
         <v>1404</v>
       </c>
@@ -16859,10 +16850,10 @@
         <v>1409</v>
       </c>
       <c r="P221" s="22" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="222" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="7" t="s">
         <v>1410</v>
       </c>
@@ -16892,10 +16883,10 @@
         <v>1414</v>
       </c>
       <c r="P222" s="21" t="s">
-        <v>1921</v>
-      </c>
-    </row>
-    <row r="223" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1917</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="7" t="s">
         <v>1415</v>
       </c>
@@ -16925,10 +16916,10 @@
         <v>1420</v>
       </c>
       <c r="P223" s="22" t="s">
-        <v>1794</v>
-      </c>
-    </row>
-    <row r="224" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="7" t="s">
         <v>1421</v>
       </c>
@@ -16961,11 +16952,11 @@
         <v>1426</v>
       </c>
       <c r="P224" s="21" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="Q224" s="7"/>
     </row>
-    <row r="225" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="7" t="s">
         <v>1427</v>
       </c>
@@ -17002,7 +16993,7 @@
       </c>
       <c r="Q225" s="7"/>
     </row>
-    <row r="226" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="7" t="s">
         <v>1432</v>
       </c>
@@ -17032,10 +17023,10 @@
         <v>1435</v>
       </c>
       <c r="P226" s="21" t="s">
-        <v>1796</v>
-      </c>
-    </row>
-    <row r="227" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="7" t="s">
         <v>1436</v>
       </c>
@@ -17061,10 +17052,10 @@
         <v>1441</v>
       </c>
       <c r="P227" s="22" t="s">
-        <v>1849</v>
-      </c>
-    </row>
-    <row r="228" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="7" t="s">
         <v>1442</v>
       </c>
@@ -17094,10 +17085,10 @@
         <v>1445</v>
       </c>
       <c r="P228" s="21" t="s">
-        <v>1813</v>
-      </c>
-    </row>
-    <row r="229" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1926</v>
+      </c>
+    </row>
+    <row r="229" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="7" t="s">
         <v>1446</v>
       </c>
@@ -17136,7 +17127,7 @@
         <v>1712</v>
       </c>
     </row>
-    <row r="230" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="7" t="s">
         <v>1453</v>
       </c>
@@ -17173,7 +17164,7 @@
       </c>
       <c r="Q230" s="7"/>
     </row>
-    <row r="231" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="7" t="s">
         <v>1459</v>
       </c>
@@ -17212,11 +17203,11 @@
         <v>1465</v>
       </c>
       <c r="P231" s="22" t="s">
-        <v>1848</v>
+        <v>1846</v>
       </c>
       <c r="Q231" s="7"/>
     </row>
-    <row r="232" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="7" t="s">
         <v>1466</v>
       </c>
@@ -17246,11 +17237,11 @@
         <v>1470</v>
       </c>
       <c r="P232" s="21" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="Q232" s="7"/>
     </row>
-    <row r="233" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="7" t="s">
         <v>1471</v>
       </c>
@@ -17288,7 +17279,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="234" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="7" t="s">
         <v>1479</v>
       </c>
@@ -17321,10 +17312,10 @@
         <v>1485</v>
       </c>
       <c r="P234" s="21" t="s">
-        <v>1910</v>
-      </c>
-    </row>
-    <row r="235" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="235" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="7" t="s">
         <v>1486</v>
       </c>
@@ -17356,11 +17347,11 @@
         <v>1491</v>
       </c>
       <c r="P235" s="22" t="s">
-        <v>1847</v>
+        <v>1845</v>
       </c>
       <c r="Q235" s="7"/>
     </row>
-    <row r="236" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="7" t="s">
         <v>1492</v>
       </c>
@@ -17393,7 +17384,7 @@
         <v>1497</v>
       </c>
     </row>
-    <row r="237" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="7" t="s">
         <v>1498</v>
       </c>
@@ -17423,10 +17414,10 @@
         <v>1503</v>
       </c>
       <c r="P237" s="22" t="s">
-        <v>1798</v>
-      </c>
-    </row>
-    <row r="238" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="7" t="s">
         <v>1504</v>
       </c>
@@ -17443,7 +17434,7 @@
         <v>757</v>
       </c>
       <c r="F238" s="7" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
       <c r="G238" s="7" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E238," ",REPT(" ",100)),100)) &amp; YEAR(C238) &amp; IFERROR(LEFT(A238,FIND(" ",A238)-1),A238)), ":", "")</f>
@@ -17456,10 +17447,10 @@
         <v>1506</v>
       </c>
       <c r="P238" s="21" t="s">
-        <v>1846</v>
-      </c>
-    </row>
-    <row r="239" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="239" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="7" t="s">
         <v>1507</v>
       </c>
@@ -17485,10 +17476,10 @@
         <v>1513</v>
       </c>
       <c r="P239" s="22" t="s">
-        <v>1845</v>
-      </c>
-    </row>
-    <row r="240" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="240" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="7" t="s">
         <v>1514</v>
       </c>
@@ -17521,11 +17512,11 @@
         <v>1518</v>
       </c>
       <c r="P240" s="21" t="s">
-        <v>1844</v>
+        <v>1842</v>
       </c>
       <c r="Q240" s="7"/>
     </row>
-    <row r="241" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="7" t="s">
         <v>1519</v>
       </c>
@@ -17542,7 +17533,7 @@
         <v>964</v>
       </c>
       <c r="F241" s="7" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="G241" s="7" t="str">
         <f>SUBSTITUTE(LOWER(TRIM(RIGHT(SUBSTITUTE(E241," ",REPT(" ",100)),100)) &amp; YEAR(C241) &amp; IFERROR(LEFT(A241,FIND(" ",A241)-1),A241)), ":", "")</f>
@@ -17558,11 +17549,11 @@
         <v>1522</v>
       </c>
       <c r="P241" s="22" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="Q241" s="7"/>
     </row>
-    <row r="242" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="7" t="s">
         <v>1523</v>
       </c>
@@ -17594,10 +17585,10 @@
         <v>1529</v>
       </c>
       <c r="P242" s="21" t="s">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="243" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="243" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="7" t="s">
         <v>1530</v>
       </c>
@@ -17633,7 +17624,7 @@
         <v>1717</v>
       </c>
     </row>
-    <row r="244" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="7" t="s">
         <v>1535</v>
       </c>
@@ -17673,7 +17664,7 @@
       </c>
       <c r="Q244" s="7"/>
     </row>
-    <row r="245" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="7" t="s">
         <v>1541</v>
       </c>
@@ -17703,7 +17694,7 @@
         <v>1546</v>
       </c>
     </row>
-    <row r="246" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="7" t="s">
         <v>1547</v>
       </c>
@@ -17736,10 +17727,10 @@
         <v>1552</v>
       </c>
       <c r="P246" s="21" t="s">
-        <v>1801</v>
-      </c>
-    </row>
-    <row r="247" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="247" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="7" t="s">
         <v>1553</v>
       </c>
@@ -17771,11 +17762,11 @@
         <v>1559</v>
       </c>
       <c r="P247" s="22" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="Q247" s="7"/>
     </row>
-    <row r="248" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="7" t="s">
         <v>1560</v>
       </c>
@@ -17805,10 +17796,10 @@
         <v>1565</v>
       </c>
       <c r="P248" s="21" t="s">
-        <v>1803</v>
-      </c>
-    </row>
-    <row r="249" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="249" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="7" t="s">
         <v>1566</v>
       </c>
@@ -17835,10 +17826,10 @@
         <v>1570</v>
       </c>
       <c r="P249" s="22" t="s">
-        <v>1804</v>
-      </c>
-    </row>
-    <row r="250" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="250" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="7" t="s">
         <v>1571</v>
       </c>
@@ -17865,10 +17856,10 @@
         <v>1574</v>
       </c>
       <c r="P250" s="21" t="s">
-        <v>1887</v>
-      </c>
-    </row>
-    <row r="251" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="251" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="7" t="s">
         <v>1575</v>
       </c>
@@ -17895,10 +17886,10 @@
         <v>1578</v>
       </c>
       <c r="P251" s="22" t="s">
-        <v>1889</v>
-      </c>
-    </row>
-    <row r="252" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1885</v>
+      </c>
+    </row>
+    <row r="252" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="7" t="s">
         <v>1579</v>
       </c>
@@ -17931,10 +17922,10 @@
         <v>1584</v>
       </c>
       <c r="P252" s="21" t="s">
-        <v>1909</v>
-      </c>
-    </row>
-    <row r="253" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="253" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="7" t="s">
         <v>1585</v>
       </c>
@@ -17963,10 +17954,10 @@
         <v>1591</v>
       </c>
       <c r="P253" s="22" t="s">
-        <v>1805</v>
-      </c>
-    </row>
-    <row r="254" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="254" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="7" t="s">
         <v>1592</v>
       </c>
@@ -17993,10 +17984,10 @@
         <v>1597</v>
       </c>
       <c r="P254" s="21" t="s">
-        <v>1806</v>
-      </c>
-    </row>
-    <row r="255" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="255" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="7" t="s">
         <v>1598</v>
       </c>
@@ -18026,10 +18017,10 @@
         <v>1601</v>
       </c>
       <c r="P255" s="22" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="256" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="256" spans="1:17" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="7" t="s">
         <v>1602</v>
       </c>
@@ -18061,10 +18052,10 @@
         <v>1608</v>
       </c>
       <c r="P256" s="21" t="s">
-        <v>1842</v>
-      </c>
-    </row>
-    <row r="257" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="257" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="7" t="s">
         <v>1609</v>
       </c>
@@ -18091,10 +18082,10 @@
         <v>1613</v>
       </c>
       <c r="P257" s="22" t="s">
-        <v>1807</v>
-      </c>
-    </row>
-    <row r="258" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="258" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="7" t="s">
         <v>1614</v>
       </c>
@@ -18124,10 +18115,10 @@
         <v>1618</v>
       </c>
       <c r="P258" s="21" t="s">
-        <v>1808</v>
-      </c>
-    </row>
-    <row r="259" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="259" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="7" t="s">
         <v>1619</v>
       </c>
@@ -18154,10 +18145,10 @@
         <v>1622</v>
       </c>
       <c r="P259" s="22" t="s">
-        <v>1843</v>
-      </c>
-    </row>
-    <row r="260" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="260" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="7" t="s">
         <v>1623</v>
       </c>
@@ -18190,10 +18181,10 @@
         <v>1630</v>
       </c>
       <c r="P260" s="21" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="261" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="261" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="7" t="s">
         <v>1631</v>
       </c>
@@ -18220,10 +18211,10 @@
         <v>1634</v>
       </c>
       <c r="P261" s="22" t="s">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="262" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1882</v>
+      </c>
+    </row>
+    <row r="262" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="7" t="s">
         <v>1635</v>
       </c>
@@ -18262,7 +18253,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="263" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="7" t="s">
         <v>1641</v>
       </c>
@@ -18279,7 +18270,7 @@
         <v>1642</v>
       </c>
       <c r="F263" s="7" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="G263" s="7" t="str">
         <f t="shared" si="5"/>
@@ -18292,10 +18283,10 @@
         <v>1644</v>
       </c>
       <c r="P263" s="22" t="s">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="264" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="264" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="7" t="s">
         <v>1645</v>
       </c>
@@ -18319,16 +18310,16 @@
         <v>farley2025liftvr</v>
       </c>
       <c r="H264" s="26" t="s">
-        <v>1919</v>
+        <v>1915</v>
       </c>
       <c r="O264" s="7" t="s">
         <v>1648</v>
       </c>
       <c r="P264" s="21" t="s">
-        <v>1840</v>
-      </c>
-    </row>
-    <row r="265" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="265" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="7" t="s">
         <v>1649</v>
       </c>
@@ -18361,10 +18352,10 @@
         <v>1654</v>
       </c>
       <c r="P265" s="22" t="s">
-        <v>1809</v>
-      </c>
-    </row>
-    <row r="266" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="266" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="7" t="s">
         <v>1655</v>
       </c>
@@ -18394,10 +18385,10 @@
         <v>1658</v>
       </c>
       <c r="P266" s="21" t="s">
-        <v>1810</v>
-      </c>
-    </row>
-    <row r="267" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="267" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="7" t="s">
         <v>1659</v>
       </c>
@@ -18430,10 +18421,10 @@
         <v>1663</v>
       </c>
       <c r="P267" s="22" t="s">
-        <v>1811</v>
-      </c>
-    </row>
-    <row r="268" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="268" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="7" t="s">
         <v>1664</v>
       </c>
@@ -18466,10 +18457,10 @@
         <v>1668</v>
       </c>
       <c r="P268" s="21" t="s">
-        <v>1812</v>
-      </c>
-    </row>
-    <row r="269" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="269" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="7" t="s">
         <v>1669</v>
       </c>
@@ -18505,10 +18496,10 @@
         <v>1672</v>
       </c>
       <c r="P269" s="22" t="s">
-        <v>1827</v>
-      </c>
-    </row>
-    <row r="270" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="270" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="7" t="s">
         <v>1673</v>
       </c>
@@ -18538,10 +18529,10 @@
         <v>1678</v>
       </c>
       <c r="P270" s="21" t="s">
-        <v>1828</v>
-      </c>
-    </row>
-    <row r="271" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="271" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="7" t="s">
         <v>1682</v>
       </c>
@@ -18577,10 +18568,10 @@
         <v>1687</v>
       </c>
       <c r="P271" s="22" t="s">
-        <v>1822</v>
-      </c>
-    </row>
-    <row r="272" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="272" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="9" t="s">
         <v>1688</v>
       </c>
@@ -18597,7 +18588,7 @@
         <v>1374</v>
       </c>
       <c r="F272" s="9" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
       <c r="G272" s="9" t="s">
         <v>1692</v>
@@ -18617,12 +18608,12 @@
         <v>1691</v>
       </c>
       <c r="P272" s="5" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="Q272" s="18"/>
       <c r="R272" s="18"/>
     </row>
-    <row r="273" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:18" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="7" t="s">
         <v>1693</v>
       </c>
@@ -18655,7 +18646,7 @@
         <v>1694</v>
       </c>
       <c r="P273" s="31" t="s">
-        <v>1839</v>
+        <v>1837</v>
       </c>
       <c r="R273" s="10" t="s">
         <v>1698</v>

</xml_diff>